<commit_message>
Luận xong Phu Thê
</commit_message>
<xml_diff>
--- a/LuanPhuThe.xlsx
+++ b/LuanPhuThe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4247FD-4F4C-4D88-990F-3FD00F12A484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3649A2-4E3D-4F02-AAF7-02A620E31157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7622" uniqueCount="3730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7656" uniqueCount="3747">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11215,6 +11215,57 @@
   </si>
   <si>
     <t>Thai Phụ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Đào Hoa, Hồng Loan, Tả Phù, Hữu Bật đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Đào Hoa, Thiên Riêu đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hồng Loan, Đào Hoa, Hóa Kỵ đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hồng Loan, Đào Hoa, Hoa Cái đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hóa Lộc, Thiên Mã, Long Trì đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hóa Lộc, Phượng Các, Long Trì đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hóa Lộc, Hồng Loan đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hóa Kỵ, Phục Binh đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hóa Kỵ, Thiên Riêu đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hồng Loan, Đào Hoa, Hóa Kỵ, Đà La đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hóa Kỵ, Địa Kiếp, Kiếp Sát đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Thất Sát, Thiên Riêu, Hỏa Tinh, Linh Tinh, Đà La đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Tham Lang, Đà La đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Thiên Tướng, Đào Hoa, Hồng Loan đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Cự Môn, Hỏa Tinh, Linh Tinh đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Tiểu Hao, Đại Hao đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Ân Quang, Thiên Quý đồng cung tại Phu Thê</t>
   </si>
 </sst>
 </file>
@@ -11753,10 +11804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3812"/>
+  <dimension ref="A1:B3830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1658" workbookViewId="0">
-      <selection activeCell="P1668" sqref="P1668"/>
+    <sheetView tabSelected="1" topLeftCell="A3800" workbookViewId="0">
+      <selection activeCell="B3830" sqref="B3830"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42250,6 +42301,142 @@
       </c>
       <c r="B3812" t="s">
         <v>3608</v>
+      </c>
+    </row>
+    <row r="3814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3814" t="s">
+        <v>3730</v>
+      </c>
+      <c r="B3814" t="s">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3815" t="s">
+        <v>3731</v>
+      </c>
+      <c r="B3815" t="s">
+        <v>3731</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3816" t="s">
+        <v>3732</v>
+      </c>
+      <c r="B3816" t="s">
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3817" t="s">
+        <v>3733</v>
+      </c>
+      <c r="B3817" t="s">
+        <v>3733</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3818" t="s">
+        <v>3734</v>
+      </c>
+      <c r="B3818" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3819" t="s">
+        <v>3735</v>
+      </c>
+      <c r="B3819" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3820" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B3820" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3821" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B3821" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3822" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B3822" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="3823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3823" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B3823" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="3824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3824" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B3824" t="s">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="3825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3825" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B3825" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="3826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3826" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B3826" t="s">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="3827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3827" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B3827" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="3828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3828" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B3828" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3829" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B3829" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3830" t="s">
+        <v>3746</v>
+      </c>
+      <c r="B3830" t="s">
+        <v>3746</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thích các phụ tinh tại phu thê trừ cá sát tinh
</commit_message>
<xml_diff>
--- a/LuanPhuThe.xlsx
+++ b/LuanPhuThe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F83800B-B977-4600-ABFB-96731DE4E670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74575A3-D793-46D3-AF54-28A25C54E24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8826" uniqueCount="4419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8876" uniqueCount="4470">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13283,6 +13283,160 @@
   <si>
     <t xml:space="preserve">Lấy nhau dễ dàng, thường gặp nhau ở xa mà nên duyên vợ chồng, rất khá 
 giả và hòa thuận. </t>
+  </si>
+  <si>
+    <t>Lộc Phượng Long</t>
+  </si>
+  <si>
+    <t>Lộc Phượng Long hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Lấy được người phối ngẫu rất giàu có</t>
+  </si>
+  <si>
+    <t>Quý Anh có Hồng Loan, Hóa Lộc đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh cưới được người vợ có của</t>
+  </si>
+  <si>
+    <t>Phục Binh, Hóa Kỵ đồng cung tại Quan Lộc đối xung với Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng ghét nhau, tìm cách bôi nhọ lẫn nhau. </t>
+  </si>
+  <si>
+    <t>Riêu Kỵ</t>
+  </si>
+  <si>
+    <t>Riêu Kỵ hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Người phối ngẫu dễ ngoại tình, loạn dâm</t>
+  </si>
+  <si>
+    <t>Kỵ Đà Hồng Đào</t>
+  </si>
+  <si>
+    <t>Kỵ Đà Hồng Đào hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Yêu nhau nhưng vẫn tìm cách lừa dối nhau. Người phối ngẫu dễ ngoại tình</t>
+  </si>
+  <si>
+    <t>Kiếp Kỵ</t>
+  </si>
+  <si>
+    <t>Kiếp Sát Kỵ</t>
+  </si>
+  <si>
+    <t>Kiếp Kỵ hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kiếp Sát Kỵ hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng hại nhau. </t>
+  </si>
+  <si>
+    <t>Sát Đà Riêu Linh Hỏa</t>
+  </si>
+  <si>
+    <t>Sát Đà Riêu Linh Hỏa hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Rất nguy hiểm đến tính mạng khi lấy người này, tuyệt đối không nên cưới</t>
+  </si>
+  <si>
+    <t>Kiếp Sát Đà Riêu Linh Hỏa</t>
+  </si>
+  <si>
+    <t>Kiếp Sát Đà Riêu Linh Hỏa hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Người phối ngẫu ham chơi, ham tửu sắc, phóng đãng</t>
+  </si>
+  <si>
+    <t>Cưới được người giàu có, hiền lành, và có ngoại hình rất đẹp</t>
+  </si>
+  <si>
+    <t>Tham Sát</t>
+  </si>
+  <si>
+    <t>Tham Sát hội chiếu tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Lấy người không hòa hợp, nhiều hình khắc</t>
+  </si>
+  <si>
+    <t>Mối lái rất nhiều nhưng vẫn khó tìm hôn phối.</t>
+  </si>
+  <si>
+    <t>Nhu cầu sinh lý của người phối ngẫu rất lớn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng bất hòa hay xa cách nhau. </t>
+  </si>
+  <si>
+    <t>Cưới xin quá dễ dàng nhưng lấy về cũng tốn kém. Người phối ngẫu có thể rất thích cờ bạc, chi tiêu hoang phí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng vì ân tình mà lấy nhau. 
+</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Tướng toạ thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Tướng toạ thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quen nhau, thường đi lại với nhau rồi mới cưới. Anh cũng sợ vợ vì vợ hay ghen</t>
+  </si>
+  <si>
+    <t>Quen nhau, thường đi lại với nhau rồi mới cưới. Chị cũng nể chồng nhưng vẫn tìm cách để bắt nạt</t>
+  </si>
+  <si>
+    <t>Quen nhau, thường qua lại với nhau rồi mới cưới</t>
+  </si>
+  <si>
+    <t>Hay có sự xích mích trong gia đình.</t>
+  </si>
+  <si>
+    <t>Thái Tuế toạ thủ tại Quan Lộc đối xung với Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gặp nhau ở nơi xa mà nên duyên vợ chồng. </t>
+  </si>
+  <si>
+    <t>Nên chậm cưới để tránh sự bất hòa hay chia ly sau này.</t>
+  </si>
+  <si>
+    <t>Vợ chồng bất hòa.</t>
+  </si>
+  <si>
+    <t>Hóa Kỵ toạ thủ tại Quan Lộc đối xung với Phu Thê</t>
+  </si>
+  <si>
+    <t>Người phối ngẫu có học thức, đỗ đạt</t>
+  </si>
+  <si>
+    <t>Người phối ngẫu khiến mình phải nể trọng, hoăc rất nghiêm khắc, có chức quyền.</t>
+  </si>
+  <si>
+    <t>Người phối ngẫu rất giàu có</t>
+  </si>
+  <si>
+    <t>Người phối ngẫu thường là con cả, nếu không cũng gánh vác vai trò thay con cả, người phối ngẫu có ngoại hình đẹp.</t>
+  </si>
+  <si>
+    <t>Thiên Khôi, Thiên Việt đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Vợ chồng sống với nhau hòa thuận, người phối ngẫu thông minh, có tài năng, khôn khéo, có học thức.</t>
+  </si>
+  <si>
+    <t>Văn Xương, Văn Khúc đồng cung tại Phu Thê</t>
   </si>
 </sst>
 </file>
@@ -13327,37 +13481,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13470,431 +13594,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14294,10 +13998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4416"/>
+  <dimension ref="A1:B4441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4384" workbookViewId="0">
-      <selection activeCell="E4409" sqref="E4409"/>
+    <sheetView tabSelected="1" topLeftCell="A4415" workbookViewId="0">
+      <selection activeCell="B4441" sqref="B4441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27401,12 +27105,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="1638" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1638" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1638" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B1638" s="1" t="s">
-        <v>113</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="1639" spans="1:2" x14ac:dyDescent="0.25">
@@ -27414,7 +27118,7 @@
         <v>114</v>
       </c>
       <c r="B1639" s="1" t="s">
-        <v>114</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="1640" spans="1:2" x14ac:dyDescent="0.25">
@@ -27422,7 +27126,7 @@
         <v>115</v>
       </c>
       <c r="B1640" s="1" t="s">
-        <v>115</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="1641" spans="1:2" x14ac:dyDescent="0.25">
@@ -27913,12 +27617,12 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="1703" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1703" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1703" s="1" t="s">
         <v>1701</v>
       </c>
       <c r="B1703" s="1" t="s">
-        <v>1701</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="1704" spans="1:2" x14ac:dyDescent="0.25">
@@ -28001,12 +27705,12 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="1714" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1714" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1714" s="1" t="s">
         <v>1712</v>
       </c>
       <c r="B1714" s="1" t="s">
-        <v>1712</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="1715" spans="1:2" x14ac:dyDescent="0.25">
@@ -28089,12 +27793,12 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="1725" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1725" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1725" s="1" t="s">
         <v>1723</v>
       </c>
       <c r="B1725" s="1" t="s">
-        <v>1723</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="1726" spans="1:2" x14ac:dyDescent="0.25">
@@ -29238,7 +28942,7 @@
         <v>1866</v>
       </c>
       <c r="B1868" s="1" t="s">
-        <v>1866</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="1869" spans="1:2" x14ac:dyDescent="0.25">
@@ -30294,7 +29998,7 @@
         <v>1998</v>
       </c>
       <c r="B2000" s="1" t="s">
-        <v>1998</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="2001" spans="1:2" x14ac:dyDescent="0.25">
@@ -30382,7 +30086,7 @@
         <v>2009</v>
       </c>
       <c r="B2011" s="1" t="s">
-        <v>2009</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="2012" spans="1:2" x14ac:dyDescent="0.25">
@@ -30470,7 +30174,7 @@
         <v>2020</v>
       </c>
       <c r="B2022" s="1" t="s">
-        <v>2020</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="2023" spans="1:2" x14ac:dyDescent="0.25">
@@ -30565,8 +30269,8 @@
       <c r="A2034" s="1" t="s">
         <v>2032</v>
       </c>
-      <c r="B2034" s="1" t="s">
-        <v>2032</v>
+      <c r="B2034" t="s">
+        <v>4461</v>
       </c>
     </row>
     <row r="2035" spans="1:2" x14ac:dyDescent="0.25">
@@ -30645,8 +30349,8 @@
       <c r="A2044" s="1" t="s">
         <v>2042</v>
       </c>
-      <c r="B2044" s="1" t="s">
-        <v>2042</v>
+      <c r="B2044" t="s">
+        <v>4460</v>
       </c>
     </row>
     <row r="2045" spans="1:2" x14ac:dyDescent="0.25">
@@ -44254,7 +43958,7 @@
         <v>3743</v>
       </c>
       <c r="B3745" s="1" t="s">
-        <v>3743</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="3746" spans="1:2" x14ac:dyDescent="0.25">
@@ -46542,7 +46246,7 @@
         <v>4029</v>
       </c>
       <c r="B4031" s="1" t="s">
-        <v>4029</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="4032" spans="1:2" x14ac:dyDescent="0.25">
@@ -47446,7 +47150,7 @@
         <v>4142</v>
       </c>
       <c r="B4144" s="1" t="s">
-        <v>4142</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="4145" spans="1:2" x14ac:dyDescent="0.25">
@@ -47974,7 +47678,7 @@
         <v>4208</v>
       </c>
       <c r="B4210" s="1" t="s">
-        <v>4208</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="4211" spans="1:2" x14ac:dyDescent="0.25">
@@ -48113,12 +47817,12 @@
         <v>4225</v>
       </c>
     </row>
-    <row r="4229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4229" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4229" s="1" t="s">
         <v>4226</v>
       </c>
       <c r="B4229" s="1" t="s">
-        <v>4226</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="4230" spans="1:2" x14ac:dyDescent="0.25">
@@ -48137,12 +47841,12 @@
         <v>4228</v>
       </c>
     </row>
-    <row r="4232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4232" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4232" s="1" t="s">
         <v>4229</v>
       </c>
       <c r="B4232" s="1" t="s">
-        <v>4229</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="4233" spans="1:2" x14ac:dyDescent="0.25">
@@ -48153,12 +47857,12 @@
         <v>4230</v>
       </c>
     </row>
-    <row r="4234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4234" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4234" s="1" t="s">
         <v>4231</v>
       </c>
       <c r="B4234" s="1" t="s">
-        <v>4231</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="4235" spans="1:2" x14ac:dyDescent="0.25">
@@ -48470,7 +48174,7 @@
         <v>4270</v>
       </c>
       <c r="B4273" s="1" t="s">
-        <v>4270</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="4274" spans="1:2" x14ac:dyDescent="0.25">
@@ -48497,12 +48201,12 @@
         <v>4273</v>
       </c>
     </row>
-    <row r="4277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4277" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4277" s="1" t="s">
         <v>4274</v>
       </c>
       <c r="B4277" s="1" t="s">
-        <v>4274</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="4278" spans="1:2" x14ac:dyDescent="0.25">
@@ -49609,61 +49313,261 @@
         <v>4418</v>
       </c>
     </row>
+    <row r="4417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4417" s="1" t="s">
+        <v>4419</v>
+      </c>
+      <c r="B4417" s="1" t="s">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="4418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4418" s="1" t="s">
+        <v>4420</v>
+      </c>
+      <c r="B4418" s="1" t="s">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="4419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4419" s="1" t="s">
+        <v>4422</v>
+      </c>
+      <c r="B4419" s="1" t="s">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="4420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4420" s="1" t="s">
+        <v>4424</v>
+      </c>
+      <c r="B4420" s="1" t="s">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="4421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4421" s="1" t="s">
+        <v>4426</v>
+      </c>
+      <c r="B4421" s="1" t="s">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="4422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4422" s="1" t="s">
+        <v>4427</v>
+      </c>
+      <c r="B4422" s="1" t="s">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="4423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4423" s="1" t="s">
+        <v>4429</v>
+      </c>
+      <c r="B4423" s="1" t="s">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="4424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4424" s="1" t="s">
+        <v>4430</v>
+      </c>
+      <c r="B4424" s="1" t="s">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="4425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4425" s="1" t="s">
+        <v>4432</v>
+      </c>
+      <c r="B4425" s="1" t="s">
+        <v>4432</v>
+      </c>
+    </row>
+    <row r="4426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4426" s="1" t="s">
+        <v>4433</v>
+      </c>
+      <c r="B4426" s="1" t="s">
+        <v>4433</v>
+      </c>
+    </row>
+    <row r="4427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4427" s="1" t="s">
+        <v>4434</v>
+      </c>
+      <c r="B4427" s="1" t="s">
+        <v>4436</v>
+      </c>
+    </row>
+    <row r="4428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4428" s="1" t="s">
+        <v>4435</v>
+      </c>
+      <c r="B4428" s="1" t="s">
+        <v>4436</v>
+      </c>
+    </row>
+    <row r="4429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4429" s="1" t="s">
+        <v>4437</v>
+      </c>
+      <c r="B4429" s="1" t="s">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="4430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4430" s="1" t="s">
+        <v>4438</v>
+      </c>
+      <c r="B4430" s="1" t="s">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4431" s="1" t="s">
+        <v>4440</v>
+      </c>
+      <c r="B4431" s="1" t="s">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="4432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4432" s="1" t="s">
+        <v>4441</v>
+      </c>
+      <c r="B4432" s="1" t="s">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4433" s="1" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B4433" s="1" t="s">
+        <v>4442</v>
+      </c>
+    </row>
+    <row r="4434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4434" s="1" t="s">
+        <v>4444</v>
+      </c>
+      <c r="B4434" s="1" t="s">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="4435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4435" s="1" t="s">
+        <v>4445</v>
+      </c>
+      <c r="B4435" s="1" t="s">
+        <v>4446</v>
+      </c>
+    </row>
+    <row r="4436" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4436" s="1" t="s">
+        <v>4452</v>
+      </c>
+      <c r="B4436" s="1" t="s">
+        <v>4455</v>
+      </c>
+    </row>
+    <row r="4437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4437" s="1" t="s">
+        <v>4453</v>
+      </c>
+      <c r="B4437" s="1" t="s">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="4438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4438" s="1" t="s">
+        <v>4458</v>
+      </c>
+      <c r="B4438" s="1" t="s">
+        <v>4457</v>
+      </c>
+    </row>
+    <row r="4439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4439" s="1" t="s">
+        <v>4462</v>
+      </c>
+      <c r="B4439" s="1" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="4440" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4440" s="1" t="s">
+        <v>4467</v>
+      </c>
+      <c r="B4440" s="1" t="s">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="4441" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4441" s="1" t="s">
+        <v>4469</v>
+      </c>
+      <c r="B4441" s="1" t="s">
+        <v>4468</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="46" priority="94"/>
-    <cfRule type="duplicateValues" dxfId="45" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="44" priority="64"/>
-    <cfRule type="duplicateValues" dxfId="43" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="42" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="41" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="40" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3831 A3894:A4189 A6734:A1048576">
-    <cfRule type="duplicateValues" dxfId="39" priority="103"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="37" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3832:A3893">
-    <cfRule type="duplicateValues" dxfId="36" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4412 A2044 A2035:B2043 A2034 A2045:B4411 A1:B2033 A4413:B1048576">
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="35" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="33" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="31" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="29" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B1631 B1:B23 B25:B84 B143 B1805:B1809 B3442:B3831 B3894:B4189 B6734:B1048576">
-    <cfRule type="duplicateValues" dxfId="28" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B3339">
-    <cfRule type="duplicateValues" dxfId="26" priority="4"/>
+  <conditionalFormatting sqref="B1810:B2033 B2045:B3339 B2035:B2043">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3832:B3893">
-    <cfRule type="duplicateValues" dxfId="25" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B4411 A4412 A4413:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích xong phu thê
</commit_message>
<xml_diff>
--- a/LuanPhuThe.xlsx
+++ b/LuanPhuThe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74575A3-D793-46D3-AF54-28A25C54E24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD634D2-D02B-4BAA-9332-C13296564336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8876" uniqueCount="4470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9054" uniqueCount="4645">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13437,6 +13437,533 @@
   </si>
   <si>
     <t>Văn Xương, Văn Khúc đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hòa hợp trắng răng đến thuở bạc đầu. Vợ chồng đều khá giả, chung hưởng giàu sang </t>
+  </si>
+  <si>
+    <t>Tử Vi, Thiên Phủ đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Tình cảm vợ chồng bình thường</t>
+  </si>
+  <si>
+    <t>Tử Vi, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Vợ chồng đều cứng cỏi, ương ngạnh. Mới lấy nhau thường hòa hợp nhưng về sau lại hay có chuyện xích mích. Cả hai đều khá giả.</t>
+  </si>
+  <si>
+    <t>Quý Chị có Tử Vi, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tử Vi, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý chị nên lấy chồng là trưởng nam, và lớn hơn tuổi mình</t>
+  </si>
+  <si>
+    <t>Quý anh nên lấy vợ là trưởng nữ</t>
+  </si>
+  <si>
+    <t>Tử Vi, Thất Sát đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mới đầu cần khó khăn, thử thách, tìm hiểu kỹ sau đó mới tiến hành hôn nhân mới tránh được hình khác, chia ly. Nên muộn lập gia đình, như thế mới được hài lòng và được hưởng phú qúy trọn đời </t>
+  </si>
+  <si>
+    <t>Tử Vi, Phá Quân đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tử Vi, Phá Quân đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Phải hình khắc hay chia ly, sống chung với nhau thì hay tranh cãi</t>
+  </si>
+  <si>
+    <t>Quý anh nên lấy vợ lớn hơn tuổi</t>
+  </si>
+  <si>
+    <t>Tử Vi, Tham Lang đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muộn lập gia đình mới mong được bách niên giai lão. Nhưng dù sao chăng nữa, trong nhà cũng hay có sự bất hòa vì một trong hai người hay ghen tuông. </t>
+  </si>
+  <si>
+    <t>Ba lần lập gia đình, người phối ngẫu hoàn cảnh khó khăn, nghèo túng</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thiên Phủ đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Nên muộn lập gia đình. Vợ chồng tính cương cường, không ai chịu ai, nhưng chung sống được với nhau đến lúc bạc đầu. Gia đình sung túc và thường có danh giá.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Vợ chồng bất hòa, nếu không tử biệt cũng sinh ly.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Thất Sát đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hình khắc hay sinh ly, nên muộn lập gia đình để tránh mấy độ buồn thương. </t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Phá Quân đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng bất hòa, hay xa cách nhau, sinh kế khó khăn. </t>
+  </si>
+  <si>
+    <t>Liêm Trinh, Tham Lang đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Vợ chồng ở với nhau hay sinh tai họa, dễ gặp nhau lại dễ bỏ nhau, nếu không cũng sớm khắc.</t>
+  </si>
+  <si>
+    <t>Chậm cưới mới được dễ dàng mọi sự và chung sống với nhau đến lúc bạc đầu</t>
+  </si>
+  <si>
+    <t>Quý Chị nên lấy chồng là con cả.</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Đồng tọa thủ cung Phu Thê ở Mão</t>
+  </si>
+  <si>
+    <t>Quý Anh nên lấy vợ là con thứ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay có sự bất hòa trong gia đình, thường phải xa cách nhau. </t>
+  </si>
+  <si>
+    <t>Dễ gặp nhau lại dễ xa nhau</t>
+  </si>
+  <si>
+    <t>Vợ chồng hay cãi lộn, nếu không tử biệt cũng sinh ly</t>
+  </si>
+  <si>
+    <t>Thiên Đồng, Thiên Lương đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sớm lập gia đình, hai người thường có họ với nhau, nếu không cũng là cung của hai gia đình đã giao du thân mật với nhau từ lâu, vợ chồng đẹp đôi và giàu sang. </t>
+  </si>
+  <si>
+    <t>Muộn lập gia đình mới tránh được chia ly.</t>
+  </si>
+  <si>
+    <t>Thiên Đồng, Cự Môn đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Bỏ nhau, nếu không cũng phải xa cách rất lâu rồi mới đoàn tụ, vợ chồng rất thông minh.</t>
+  </si>
+  <si>
+    <t>Nên muộn lập gia đình, và lấy người bằng tuổi, hoặc gần bằng tuổi nhau, bạn được nhờ người hôn phối nhiều vì người đó có nhiều tiền tài.</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thiên Phủ đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng đôi khi có sự bất hòa, nhưng chung hưởng giàu sang đến lúc bạc đầu. </t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Vũ Khúc, Thiên Tướng đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh lấy được vợ đảm đang, tài giỏi và giàu.</t>
+  </si>
+  <si>
+    <t>Quý chị lấy được chồng hiền và sang</t>
+  </si>
+  <si>
+    <t>Cả hai đều cương cường, lúc trẻ hòa thuận, về sau hay xích mích nhưng đều được hưởng phú qúy trọn vẹn</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Tham Lang đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Nên muộn lập gia đình, vợ chồng phải chênh lệch nhau nhiều tuổi. Cả hai đều tài giỏi đảm đang nhưng nếu sớm đường hôn phối tất bị hình khắc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Phá Quân đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Vợ chồng đều thao lược nhưng nếu sớm gặp nhau tất phải hình khắc và ít nhất là hai lần lập gia đình.</t>
+  </si>
+  <si>
+    <t>Vũ Khúc, Thất Sát đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hình khắc nhau rất thê thẳm, vợ chồng chung sống với nhauhay sinh tai họa, để rồi xa cách hay hay một sống một chết. </t>
+  </si>
+  <si>
+    <t>Vợ chồng hợp chung sống trong cảnh phú qúy vinh hiển cho đến lúc đầu bạc răng long</t>
+  </si>
+  <si>
+    <t>Việc cưới xin hay trắc trở, có muộn đường hôn phối mới tránh được những sự chẳng lành.</t>
+  </si>
+  <si>
+    <t>Vợ chồng hay có sự bất hòa, nhưng chung sống được với nhau trong cảnh giàu sang cho đến lúc mãn chiều xế bóng.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muộn lập gia đình, may ra mới tránh được sự chia ly. </t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Dương, Thái Âm đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Dương, Thái Âm đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Nên muộn đường hôn phối, nếu không tất phải xa nhau nhưng cả hai đều qúy hiển, và thường nể sợ chồng</t>
+  </si>
+  <si>
+    <t>Nên muộn đường hôn phối, nếu không tất phải xa nhau nhưng cả hai đều qúy hiển, và thường nể sợ vợ</t>
+  </si>
+  <si>
+    <t>Sớm lập gia đình, vợ chồng đều cương cường, nhưng chung sống được với nhau, cả hai đều có tài và khá giả.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nên muộn lập gia đình, cả hai không hợp tính nhau </t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ, Thiên Lương đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Cơ, Thiên Lương đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Sớm gặp người hiền lương, lấy nhau dễ dàng, làm ăn khá giả và thường là người quen thuộc trước hay có họ hàng xa với nhau, và sẽ lấy được chồng hiền và hòa hợp cho đến lúc mãn chiều xế bóng</t>
+  </si>
+  <si>
+    <t>Sớm gặp người hiền lương, lấy nhau dễ dàng, làm ăn khá giả và thường là người quen thuộc trước hay có họ hàng xa với nhau, và sẽ lấy được vợ đẹp và hòa hợp cho đến lúc mãn chiều xế bóng</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ, Cự Môn đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Cơ, Cự Môn đồng cung tại Phu Thê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quý chị lấy chồng tài giỏi, có danh chức. nhưng nên muộn đường hôn phối. Nếu không tất hay xảy ra những sự tranh chấp bất hòa, dễ đi đến chỗ chia ly. </t>
+  </si>
+  <si>
+    <t>Quý anh lấy vợ đẹp, giàu sang nhưng nên muộn đường hôn phối. Nếu không tất hay xảy ra những sự tranh chấp bất hòa, dễ đi đến chỗ chia ly.</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ, Thái Âm đồng cung tại Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Cơ, Thái Âm đồng cung tại Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ, Thái Âm đồng cung tại Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Cơ, Thái Âm đồng cung tại Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t>Vợ chồng đều tài giỏi, khá giả, lấy nhau sớm</t>
+  </si>
+  <si>
+    <t>Thường gặp trở ngại trong việc cưới hỏi, nên muộn đường hôn phối để tránh những sự bất hòa hay xa cách nhau, cả hai đều có tài.</t>
+  </si>
+  <si>
+    <t>Thường gặp trở ngại trong việc cưới hỏi, nên muộn đường hôn phối để tránh những sự bất hòa hay xa cách nhau, cả hai đều có tài, quý anh hay sợ vợ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng khá giả, hòa thuận đến lúc đầu bạc. </t>
+  </si>
+  <si>
+    <t>Vợ chồng chung sống sung túc, nhưng hay cãi lộn</t>
+  </si>
+  <si>
+    <t>Vợ chồng đều qúy hiển, lấy nhau sớm, hòa thuận cho đến lúc đầu bạc. Người phối ngẫu giàu có, danh giá.</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm tọa thủ cung Phu Thê ở Dậu</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm tọa thủ cung Phu Thê ở Tuất</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm tọa thủ cung Phu Thê ở Hợi</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm tọa thủ cung Phu Thê ở Dậu</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm tọa thủ cung Phu Thê ở Tuất</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm tọa thủ cung Phu Thê ở Hợi</t>
+  </si>
+  <si>
+    <t>Quý anh lấy được vợ đẹp và giàu sang, thường nể vợ và đôi khi nhờ vợ mới có danh giá, của cải</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quý chị lấy được chồng hiền, đáng ngôi mệnh phụ đường đường. </t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm tọa thủ cung Phu Thê ở Mão</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm tọa thủ cung Phu Thê ở Thìn</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm tọa thủ cung Phu Thê ở Tỵ</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm tọa thủ cung Phu Thê ở Mão</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm tọa thủ cung Phu Thê ở Thìn</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm tọa thủ cung Phu Thê ở Tỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng hay bất hòa, lấy phải chồng bần tiện, bất nhân. Trong lúc cưới xin, gặp nhiều trở ngại, nên muộn đường hôn phối để cố tránh những nỗi buồn khổ, chia ly. </t>
+  </si>
+  <si>
+    <t>Quý Chị có Thái Âm, Thiên Đồng đồng cung tại Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thái Âm, Thiên Đồng đồng cung tại Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng hay bất hòa, lấy vợ lăng loàn, dâm đăng. Trong lúc cưới xin, gặp nhiều trở
+ngại, nên muộn đường hôn phối để cố tránh những nỗi buồn khổ, chia ly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng hay bất hòa, lấy vợ lăng loàn, dâm đăng, quý anh hay nể vợ và được nhờ vợ nhiều. Trong lúc cưới xin, gặp nhiều trở ngại, nên muộn đường hôn phối để cố tránh những nỗi buồn khổ, chia ly. </t>
+  </si>
+  <si>
+    <t>Vợ chồng đều tài giỏi, khá giả, lấy nhau sớm, quý anh hay nể vợ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Tham Lang tọa thủ cung Phu Thê ở Thìn</t>
+  </si>
+  <si>
+    <t>Quý Chị có Tham Lang tọa thủ cung Phu Thê ở Tuất</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tham Lang tọa thủ cung Phu Thê ở Thìn</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tham Lang tọa thủ cung Phu Thê ở Tuất</t>
+  </si>
+  <si>
+    <t>Quý anh lấy được vợ giàu, tài giỏi nhưng hay ghen. Nên lấy muộn để tránh hình khắc chia ly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quý chị lấy được chồng sang nhưng hay chơi bời. Nên muộn lập gia đình để tránh những
+hình khắc hay chia ly. </t>
+  </si>
+  <si>
+    <t>Quý Chị có Tham Lang tọa thủ cung Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý Chị có Tham Lang tọa thủ cung Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tham Lang tọa thủ cung Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tham Lang tọa thủ cung Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t>Quý anh lấy phải vợ hay ghen và dâm đãng.  Nên muộn đường hôn phối, vì dễ gặp nhau để rồi lại dễ xa nhau, hay hình khắc nhau.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quý chị lấy phải chồng nghèo hay hoang đãng lưu manh. Nên muộn đường hôn phối, vì dễ gặp nhau để rồi lại dễ xa nhau, hay hình khắc nhau. </t>
+  </si>
+  <si>
+    <t>Quý Chị có Tham Lang tọa thủ cung Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t>Quý Chị có Tham Lang tọa thủ cung Phu Thê ở Ngọ</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tham Lang tọa thủ cung Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t>Quý Anh có Tham Lang tọa thủ cung Phu Thê ở Ngọ</t>
+  </si>
+  <si>
+    <t>Vợ chồng đẹp đôi, đều qúy hiển, nhưng hay bất hòa.</t>
+  </si>
+  <si>
+    <t>Vợ chồng bỏ nhau, hai hay ba lần lập gia đình.</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh có Thiên Tướng tọa thủ cung Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh hay nể vợ và vợ thường là con gái trưởng</t>
+  </si>
+  <si>
+    <t>Quý chị hay tìm cách lấn át chồng, và chồng thường là con cả.</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Phu Thê ở Tỵ</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Phu Thê ở Hợi</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Phu Thê ở Sửu</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Phu Thê ở Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muộn đường hôn phối đế tránh sự bất hòa hay xa cách. Quý chị lấy được chống có danh chức và giỏi dang. Nếu hai người có họ xa với nhau lại càng tốt đôi. </t>
+  </si>
+  <si>
+    <t>Quý anh có Thiên Tướng tọa thủ cung Phu Thê ở Tỵ</t>
+  </si>
+  <si>
+    <t>Quý anh có Thiên Tướng tọa thủ cung Phu Thê ở Hợi</t>
+  </si>
+  <si>
+    <t>Quý anh có Thiên Tướng tọa thủ cung Phu Thê ở Sửu</t>
+  </si>
+  <si>
+    <t>Quý anh có Thiên Tướng tọa thủ cung Phu Thê ở Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muộn đường hôn phối đế tránh sự bất hòa hay xa cách. Quý anh lấy vợ được đẹp, khôn ngoan, có tài đảm đang, con nhà khá giả. Quý anh nên hơn vợ nhiều tuổi, nếu hai người có họ xa với nhau lại càng tốt đôi. </t>
+  </si>
+  <si>
+    <t>Nhiều trở ngại trong việc cưới xin. Nếu muộn lập gia đình mới tránh được mọi hình khắc, chia ly.</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Lương tọa thủ cung Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh có Thiên Lương tọa thủ cung Phu Thê</t>
+  </si>
+  <si>
+    <t>Người chồng của quý chị rất phong lựu</t>
+  </si>
+  <si>
+    <t>Người vợ của quý anh rất đẹp gái</t>
+  </si>
+  <si>
+    <t>Vợ chồng lấy nhau sớm và dễ dàng, cả hai đều qúy hiển, người phối ngẫu của bạn là con cả.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng dễ gặp nhau lại dễ xa nhau. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vợ chồng hợp chung sống trong cảnh phú qúy vinh hiển cho đến lúc đầu bạc răng long. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Việc cưới xin hay trắc trở, có muộn đường hôn phối mới tránh được những sự chẳng lành. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muộn đường hôn phối, quý chị lấy chồng danh giá và thường là con trai trưởng, cả hai đều cương cường. </t>
+  </si>
+  <si>
+    <t>Quý anh có Thất Sát tọa thủ cung Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý anh có Thất Sát tọa thủ cung Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muộn đường hôn phối, quý anh lấy vợ tài giỏi nhưng hay ghen và thường là con gái trưởng, cả hai đều cương cường. </t>
+  </si>
+  <si>
+    <t>Muộn đường hôn phối, quý chị lấy chồng danh giá và thường là con trai trưởng, cả hai đều cương cường. Vợ chồng hay bất hòa, nếu sớm lập gia đình tất phải hình khắc hay chia ly.</t>
+  </si>
+  <si>
+    <t>Quý anh có Thất Sát tọa thủ cung Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t>Muộn đường hôn phối, quý anh lấy vợ tài giỏi nhưng hay ghen và thường là con gái trưởng, cả hai đều cương cường. Vợ chồng hay bất hòa, nếu sớm lập gia đình tất phải hình khắc hay chia ly.</t>
+  </si>
+  <si>
+    <t>Quý anh có Thất Sát tọa thủ cung Phu Thê ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phải hai ba lần lập gia đình, rất nhiều tai ương xảy ra trong cuộc sống chung </t>
+  </si>
+  <si>
+    <t>Quý chị có Phá Quân tọa thủ cung Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh có Phá Quân tọa thủ cung Phu Thê</t>
+  </si>
+  <si>
+    <t>Quý anh lấy vợ hay ghen</t>
+  </si>
+  <si>
+    <t>Quý chị lấy chồng bất nghĩa</t>
+  </si>
+  <si>
+    <t>Tuy vợ chồng khá giả nhưng nên muộn đường hôn phối, nếu không trong đời tất có phen phải xa cách nhau.</t>
+  </si>
+  <si>
+    <t>Quý chị có Phá Quân tọa thủ cung Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý chị có Phá Quân tọa thủ cung Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t>Quý anh có Phá Quân tọa thủ cung Phu Thê ở Dần</t>
+  </si>
+  <si>
+    <t>Quý anh có Phá Quân tọa thủ cung Phu Thê ở Thân</t>
+  </si>
+  <si>
+    <t>Hình khắc không thế tránh được,  ấy phải chồng bất nghĩa, hoang đàng, chơi bời.</t>
+  </si>
+  <si>
+    <t>Hình khắc không thế tránh được, trai lấy phải vợ bất nhân, dâm đãng và lăng loàn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nên muộn lập gia đình, nếu không tất phải hai ba lần chắp nối đường tơ. </t>
+  </si>
+  <si>
+    <t>Kình Đà Hỏa Linh sáng tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kình Đà Hỏa Linh tối tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Địa Không, Địa Kiếp sáng tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Địa Không, Địa Kiếp tối tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Linh Tinh sáng tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Linh Tinh tối tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La sáng tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La tối tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Hay bất hòa, nếu cô phải chia ly cũng chi trong một thời gian ngắn.</t>
+  </si>
+  <si>
+    <t>Cưới xin khó khăn, sự hình khắc chia ly càng dễ xảy đến, hung họa càng nhiều thêm</t>
   </si>
 </sst>
 </file>
@@ -13481,7 +14008,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13998,10 +14545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4441"/>
+  <dimension ref="A1:B4527"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4415" workbookViewId="0">
-      <selection activeCell="B4441" sqref="B4441"/>
+    <sheetView tabSelected="1" topLeftCell="A4510" workbookViewId="0">
+      <selection activeCell="G4530" sqref="G4530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23054,7 +23601,7 @@
         <v>1261</v>
       </c>
       <c r="B1131" s="1" t="s">
-        <v>1261</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24713,12 +25260,12 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="1339" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1339" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1339" s="1" t="s">
         <v>1450</v>
       </c>
       <c r="B1339" s="1" t="s">
-        <v>1450</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="1340" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -24753,12 +25300,12 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="1344" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1344" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1344" s="1" t="s">
         <v>1455</v>
       </c>
       <c r="B1344" s="1" t="s">
-        <v>1455</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="1345" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -24793,12 +25340,12 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="1349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1349" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1349" s="1" t="s">
         <v>1460</v>
       </c>
       <c r="B1349" s="1" t="s">
-        <v>1460</v>
+        <v>4618</v>
       </c>
     </row>
     <row r="1350" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -24833,12 +25380,12 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="1354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1354" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1354" s="1" t="s">
         <v>1465</v>
       </c>
       <c r="B1354" s="1" t="s">
-        <v>1465</v>
+        <v>4618</v>
       </c>
     </row>
     <row r="1355" spans="1:2" x14ac:dyDescent="0.25">
@@ -26374,7 +26921,7 @@
         <v>27</v>
       </c>
       <c r="B1546" s="1" t="s">
-        <v>27</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1547" spans="1:2" x14ac:dyDescent="0.25">
@@ -26449,12 +26996,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1556" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1556" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1556" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B1556" s="1" t="s">
-        <v>37</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="1557" spans="1:2" x14ac:dyDescent="0.25">
@@ -27094,7 +27641,7 @@
         <v>111</v>
       </c>
       <c r="B1636" s="1" t="s">
-        <v>111</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1637" spans="1:2" x14ac:dyDescent="0.25">
@@ -27166,7 +27713,7 @@
         <v>120</v>
       </c>
       <c r="B1645" s="1" t="s">
-        <v>120</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1646" spans="1:2" x14ac:dyDescent="0.25">
@@ -27281,6 +27828,14 @@
         <v>1658</v>
       </c>
     </row>
+    <row r="1660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1660" s="1" t="s">
+        <v>4500</v>
+      </c>
+      <c r="B1660" s="1" t="s">
+        <v>4501</v>
+      </c>
+    </row>
     <row r="1661" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1661" s="1" t="s">
         <v>1659</v>
@@ -33742,7 +34297,7 @@
         <v>2345</v>
       </c>
       <c r="B2468" s="1" t="s">
-        <v>2345</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="2469" spans="1:2" x14ac:dyDescent="0.25">
@@ -33790,7 +34345,7 @@
         <v>2351</v>
       </c>
       <c r="B2474" s="1" t="s">
-        <v>2351</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="2475" spans="1:2" x14ac:dyDescent="0.25">
@@ -33838,7 +34393,7 @@
         <v>2357</v>
       </c>
       <c r="B2480" s="1" t="s">
-        <v>2357</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="2481" spans="1:2" x14ac:dyDescent="0.25">
@@ -33846,7 +34401,7 @@
         <v>2358</v>
       </c>
       <c r="B2481" s="1" t="s">
-        <v>2358</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="2482" spans="1:2" x14ac:dyDescent="0.25">
@@ -33873,28 +34428,28 @@
         <v>2361</v>
       </c>
     </row>
-    <row r="2485" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2485" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2485" s="1" t="s">
         <v>2362</v>
       </c>
       <c r="B2485" s="1" t="s">
-        <v>2362</v>
-      </c>
-    </row>
-    <row r="2486" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2486" s="1" t="s">
         <v>2363</v>
       </c>
       <c r="B2486" s="1" t="s">
-        <v>2363</v>
-      </c>
-    </row>
-    <row r="2487" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2487" s="1" t="s">
         <v>2364</v>
       </c>
       <c r="B2487" s="1" t="s">
-        <v>2364</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="2488" spans="1:2" x14ac:dyDescent="0.25">
@@ -33926,15 +34481,15 @@
         <v>2368</v>
       </c>
       <c r="B2491" s="1" t="s">
-        <v>2368</v>
-      </c>
-    </row>
-    <row r="2492" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2492" s="1" t="s">
         <v>2369</v>
       </c>
       <c r="B2492" s="1" t="s">
-        <v>2369</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="2493" spans="1:2" x14ac:dyDescent="0.25">
@@ -33958,7 +34513,7 @@
         <v>2372</v>
       </c>
       <c r="B2495" s="1" t="s">
-        <v>2372</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="2496" spans="1:2" x14ac:dyDescent="0.25">
@@ -33966,7 +34521,7 @@
         <v>2373</v>
       </c>
       <c r="B2496" s="1" t="s">
-        <v>2373</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="2497" spans="1:2" x14ac:dyDescent="0.25">
@@ -33974,7 +34529,7 @@
         <v>2374</v>
       </c>
       <c r="B2497" s="1" t="s">
-        <v>2374</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="2498" spans="1:2" x14ac:dyDescent="0.25">
@@ -33982,7 +34537,7 @@
         <v>2375</v>
       </c>
       <c r="B2498" s="1" t="s">
-        <v>2375</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="2499" spans="1:2" x14ac:dyDescent="0.25">
@@ -34001,28 +34556,28 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="2501" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2501" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2501" s="1" t="s">
         <v>2378</v>
       </c>
       <c r="B2501" s="1" t="s">
-        <v>2378</v>
-      </c>
-    </row>
-    <row r="2502" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2502" s="1" t="s">
         <v>2379</v>
       </c>
       <c r="B2502" s="1" t="s">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="2503" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2503" s="1" t="s">
         <v>2380</v>
       </c>
       <c r="B2503" s="1" t="s">
-        <v>2380</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="2504" spans="1:2" x14ac:dyDescent="0.25">
@@ -34057,12 +34612,12 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="2508" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2508" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2508" s="1" t="s">
         <v>2385</v>
       </c>
       <c r="B2508" s="1" t="s">
-        <v>2385</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2509" spans="1:2" x14ac:dyDescent="0.25">
@@ -34105,12 +34660,12 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="2514" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2514" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2514" s="1" t="s">
         <v>2391</v>
       </c>
       <c r="B2514" s="1" t="s">
-        <v>2391</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="2515" spans="1:2" x14ac:dyDescent="0.25">
@@ -34150,7 +34705,7 @@
         <v>2396</v>
       </c>
       <c r="B2519" s="1" t="s">
-        <v>2396</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="2520" spans="1:2" x14ac:dyDescent="0.25">
@@ -34158,7 +34713,7 @@
         <v>2397</v>
       </c>
       <c r="B2520" s="1" t="s">
-        <v>2397</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="2521" spans="1:2" x14ac:dyDescent="0.25">
@@ -34166,7 +34721,7 @@
         <v>2398</v>
       </c>
       <c r="B2521" s="1" t="s">
-        <v>2398</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="2522" spans="1:2" x14ac:dyDescent="0.25">
@@ -34198,7 +34753,7 @@
         <v>2402</v>
       </c>
       <c r="B2525" s="1" t="s">
-        <v>2402</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="2526" spans="1:2" x14ac:dyDescent="0.25">
@@ -34206,7 +34761,7 @@
         <v>2403</v>
       </c>
       <c r="B2526" s="1" t="s">
-        <v>2403</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="2527" spans="1:2" x14ac:dyDescent="0.25">
@@ -34238,7 +34793,7 @@
         <v>2407</v>
       </c>
       <c r="B2530" s="1" t="s">
-        <v>2407</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="2531" spans="1:2" x14ac:dyDescent="0.25">
@@ -34286,7 +34841,7 @@
         <v>2413</v>
       </c>
       <c r="B2536" s="1" t="s">
-        <v>2413</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="2537" spans="1:2" x14ac:dyDescent="0.25">
@@ -34326,7 +34881,7 @@
         <v>2418</v>
       </c>
       <c r="B2541" s="1" t="s">
-        <v>2418</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="2542" spans="1:2" x14ac:dyDescent="0.25">
@@ -34342,7 +34897,7 @@
         <v>2420</v>
       </c>
       <c r="B2543" s="1" t="s">
-        <v>2420</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="2544" spans="1:2" x14ac:dyDescent="0.25">
@@ -34366,7 +34921,7 @@
         <v>2423</v>
       </c>
       <c r="B2546" s="1" t="s">
-        <v>2423</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="2547" spans="1:2" x14ac:dyDescent="0.25">
@@ -34382,7 +34937,7 @@
         <v>2425</v>
       </c>
       <c r="B2548" s="1" t="s">
-        <v>2425</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="2549" spans="1:2" x14ac:dyDescent="0.25">
@@ -34398,7 +34953,7 @@
         <v>2427</v>
       </c>
       <c r="B2550" s="1" t="s">
-        <v>2427</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="2551" spans="1:2" x14ac:dyDescent="0.25">
@@ -34473,12 +35028,12 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="2560" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2560" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2560" s="1" t="s">
         <v>2437</v>
       </c>
       <c r="B2560" s="1" t="s">
-        <v>2437</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="2561" spans="1:2" x14ac:dyDescent="0.25">
@@ -34598,7 +35153,7 @@
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>2452</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="2576" spans="1:2" x14ac:dyDescent="0.25">
@@ -34630,7 +35185,7 @@
         <v>2456</v>
       </c>
       <c r="B2579" s="1" t="s">
-        <v>2456</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="2580" spans="1:2" x14ac:dyDescent="0.25">
@@ -34638,7 +35193,7 @@
         <v>2457</v>
       </c>
       <c r="B2580" s="1" t="s">
-        <v>2457</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="2581" spans="1:2" x14ac:dyDescent="0.25">
@@ -34646,7 +35201,7 @@
         <v>2458</v>
       </c>
       <c r="B2581" s="1" t="s">
-        <v>2458</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="2582" spans="1:2" x14ac:dyDescent="0.25">
@@ -34678,7 +35233,7 @@
         <v>2462</v>
       </c>
       <c r="B2585" s="1" t="s">
-        <v>2462</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="2586" spans="1:2" x14ac:dyDescent="0.25">
@@ -34686,7 +35241,7 @@
         <v>2463</v>
       </c>
       <c r="B2586" s="1" t="s">
-        <v>2463</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="2587" spans="1:2" x14ac:dyDescent="0.25">
@@ -34713,12 +35268,12 @@
         <v>2466</v>
       </c>
     </row>
-    <row r="2590" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2590" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2590" s="1" t="s">
         <v>2467</v>
       </c>
       <c r="B2590" s="1" t="s">
-        <v>2467</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="2591" spans="1:2" x14ac:dyDescent="0.25">
@@ -34777,12 +35332,12 @@
         <v>2474</v>
       </c>
     </row>
-    <row r="2598" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2598" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2598" s="1" t="s">
         <v>2475</v>
       </c>
       <c r="B2598" s="1" t="s">
-        <v>2475</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="2599" spans="1:2" x14ac:dyDescent="0.25">
@@ -34822,15 +35377,15 @@
         <v>2480</v>
       </c>
       <c r="B2603" s="1" t="s">
-        <v>2480</v>
-      </c>
-    </row>
-    <row r="2604" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2604" s="1" t="s">
         <v>2481</v>
       </c>
       <c r="B2604" s="1" t="s">
-        <v>2481</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="2605" spans="1:2" x14ac:dyDescent="0.25">
@@ -34870,7 +35425,7 @@
         <v>2486</v>
       </c>
       <c r="B2609" s="1" t="s">
-        <v>2486</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="2610" spans="1:2" x14ac:dyDescent="0.25">
@@ -34910,7 +35465,7 @@
         <v>2491</v>
       </c>
       <c r="B2614" s="1" t="s">
-        <v>2491</v>
+        <v>4622</v>
       </c>
     </row>
     <row r="2615" spans="1:2" x14ac:dyDescent="0.25">
@@ -34958,7 +35513,7 @@
         <v>2497</v>
       </c>
       <c r="B2620" s="1" t="s">
-        <v>2497</v>
+        <v>4622</v>
       </c>
     </row>
     <row r="2621" spans="1:2" x14ac:dyDescent="0.25">
@@ -34969,12 +35524,12 @@
         <v>2498</v>
       </c>
     </row>
-    <row r="2622" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2622" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2622" s="1" t="s">
         <v>2499</v>
       </c>
       <c r="B2622" s="1" t="s">
-        <v>2499</v>
+        <v>4627</v>
       </c>
     </row>
     <row r="2623" spans="1:2" x14ac:dyDescent="0.25">
@@ -35006,7 +35561,7 @@
         <v>2503</v>
       </c>
       <c r="B2626" s="1" t="s">
-        <v>2503</v>
+        <v>4634</v>
       </c>
     </row>
     <row r="2627" spans="1:2" x14ac:dyDescent="0.25">
@@ -35017,12 +35572,12 @@
         <v>2504</v>
       </c>
     </row>
-    <row r="2628" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2628" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2628" s="1" t="s">
         <v>2505</v>
       </c>
       <c r="B2628" s="1" t="s">
-        <v>2505</v>
+        <v>4627</v>
       </c>
     </row>
     <row r="2629" spans="1:2" x14ac:dyDescent="0.25">
@@ -35054,7 +35609,7 @@
         <v>2509</v>
       </c>
       <c r="B2632" s="1" t="s">
-        <v>2509</v>
+        <v>4634</v>
       </c>
     </row>
     <row r="2633" spans="1:2" x14ac:dyDescent="0.25">
@@ -38041,12 +38596,12 @@
         <v>2882</v>
       </c>
     </row>
-    <row r="3006" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3006" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3006" s="1" t="s">
         <v>2883</v>
       </c>
       <c r="B3006" s="1" t="s">
-        <v>2883</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="3007" spans="1:2" x14ac:dyDescent="0.25">
@@ -38238,7 +38793,7 @@
         <v>2907</v>
       </c>
       <c r="B3030" s="1" t="s">
-        <v>2907</v>
+        <v>4612</v>
       </c>
     </row>
     <row r="3031" spans="1:2" x14ac:dyDescent="0.25">
@@ -38281,12 +38836,12 @@
         <v>2912</v>
       </c>
     </row>
-    <row r="3036" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3036" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3036" s="1" t="s">
         <v>2913</v>
       </c>
       <c r="B3036" s="1" t="s">
-        <v>2913</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="3037" spans="1:2" x14ac:dyDescent="0.25">
@@ -47777,1649 +48332,1665 @@
         <v>4220</v>
       </c>
     </row>
+    <row r="4223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4223" s="1" t="s">
+        <v>4221</v>
+      </c>
+      <c r="B4223" s="1" t="s">
+        <v>4221</v>
+      </c>
+    </row>
     <row r="4224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4224" s="1" t="s">
-        <v>4221</v>
+        <v>4222</v>
       </c>
       <c r="B4224" s="1" t="s">
-        <v>4221</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="4225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4225" s="1" t="s">
-        <v>4222</v>
+        <v>4223</v>
       </c>
       <c r="B4225" s="1" t="s">
-        <v>4222</v>
+        <v>4223</v>
       </c>
     </row>
     <row r="4226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4226" s="1" t="s">
-        <v>4223</v>
+        <v>4224</v>
       </c>
       <c r="B4226" s="1" t="s">
-        <v>4223</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="4227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4227" s="1" t="s">
-        <v>4224</v>
+        <v>4225</v>
       </c>
       <c r="B4227" s="1" t="s">
-        <v>4224</v>
-      </c>
-    </row>
-    <row r="4228" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4225</v>
+      </c>
+    </row>
+    <row r="4228" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4228" s="1" t="s">
-        <v>4225</v>
+        <v>4226</v>
       </c>
       <c r="B4228" s="1" t="s">
-        <v>4225</v>
-      </c>
-    </row>
-    <row r="4229" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="4229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4229" s="1" t="s">
-        <v>4226</v>
+        <v>4227</v>
       </c>
       <c r="B4229" s="1" t="s">
-        <v>4468</v>
+        <v>4227</v>
       </c>
     </row>
     <row r="4230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4230" s="1" t="s">
-        <v>4227</v>
+        <v>4228</v>
       </c>
       <c r="B4230" s="1" t="s">
-        <v>4227</v>
-      </c>
-    </row>
-    <row r="4231" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4228</v>
+      </c>
+    </row>
+    <row r="4231" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4231" s="1" t="s">
-        <v>4228</v>
+        <v>4229</v>
       </c>
       <c r="B4231" s="1" t="s">
-        <v>4228</v>
-      </c>
-    </row>
-    <row r="4232" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4451</v>
+      </c>
+    </row>
+    <row r="4232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4232" s="1" t="s">
-        <v>4229</v>
+        <v>4230</v>
       </c>
       <c r="B4232" s="1" t="s">
-        <v>4451</v>
-      </c>
-    </row>
-    <row r="4233" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4230</v>
+      </c>
+    </row>
+    <row r="4233" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4233" s="1" t="s">
-        <v>4230</v>
+        <v>4231</v>
       </c>
       <c r="B4233" s="1" t="s">
-        <v>4230</v>
-      </c>
-    </row>
-    <row r="4234" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="4234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4234" s="1" t="s">
-        <v>4231</v>
+        <v>4232</v>
       </c>
       <c r="B4234" s="1" t="s">
-        <v>4450</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="4235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4235" s="1" t="s">
-        <v>4232</v>
+        <v>4233</v>
       </c>
       <c r="B4235" s="1" t="s">
-        <v>4232</v>
+        <v>4233</v>
       </c>
     </row>
     <row r="4236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4236" s="1" t="s">
-        <v>4233</v>
+        <v>4234</v>
       </c>
       <c r="B4236" s="1" t="s">
-        <v>4233</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="4237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4237" s="1" t="s">
-        <v>4234</v>
+        <v>4235</v>
       </c>
       <c r="B4237" s="1" t="s">
-        <v>4234</v>
+        <v>4235</v>
       </c>
     </row>
     <row r="4238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4238" s="1" t="s">
-        <v>4235</v>
+        <v>4236</v>
       </c>
       <c r="B4238" s="1" t="s">
-        <v>4235</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="4239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4239" s="1" t="s">
-        <v>4236</v>
+        <v>4237</v>
       </c>
       <c r="B4239" s="1" t="s">
-        <v>4236</v>
+        <v>4237</v>
       </c>
     </row>
     <row r="4240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4240" s="1" t="s">
-        <v>4237</v>
+        <v>4238</v>
       </c>
       <c r="B4240" s="1" t="s">
-        <v>4237</v>
-      </c>
-    </row>
-    <row r="4241" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4238</v>
+      </c>
+    </row>
+    <row r="4241" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4241" s="1" t="s">
-        <v>4238</v>
+        <v>4239</v>
       </c>
       <c r="B4241" s="1" t="s">
-        <v>4238</v>
-      </c>
-    </row>
-    <row r="4242" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4239</v>
+      </c>
+    </row>
+    <row r="4242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4242" s="1" t="s">
-        <v>4239</v>
+        <v>4240</v>
       </c>
       <c r="B4242" s="1" t="s">
-        <v>4239</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="4243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4243" s="1" t="s">
-        <v>4240</v>
+        <v>4241</v>
       </c>
       <c r="B4243" s="1" t="s">
-        <v>4240</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="4244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4244" s="1" t="s">
-        <v>4241</v>
+        <v>4242</v>
       </c>
       <c r="B4244" s="1" t="s">
-        <v>4241</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="4245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4245" s="1" t="s">
-        <v>4242</v>
+        <v>4243</v>
       </c>
       <c r="B4245" s="1" t="s">
-        <v>4242</v>
+        <v>4243</v>
       </c>
     </row>
     <row r="4246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4246" s="1" t="s">
-        <v>4243</v>
+        <v>4244</v>
       </c>
       <c r="B4246" s="1" t="s">
-        <v>4243</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="4247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4247" s="1" t="s">
-        <v>4244</v>
+        <v>4245</v>
       </c>
       <c r="B4247" s="1" t="s">
-        <v>4244</v>
+        <v>4245</v>
       </c>
     </row>
     <row r="4248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4248" s="1" t="s">
-        <v>4245</v>
+        <v>4246</v>
       </c>
       <c r="B4248" s="1" t="s">
-        <v>4245</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="4249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4249" s="1" t="s">
-        <v>4246</v>
+        <v>4247</v>
       </c>
       <c r="B4249" s="1" t="s">
-        <v>4246</v>
+        <v>4247</v>
       </c>
     </row>
     <row r="4250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4250" s="1" t="s">
-        <v>4247</v>
+        <v>4248</v>
       </c>
       <c r="B4250" s="1" t="s">
-        <v>4247</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="4251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4251" s="1" t="s">
-        <v>4248</v>
+        <v>4249</v>
       </c>
       <c r="B4251" s="1" t="s">
-        <v>4248</v>
+        <v>4249</v>
       </c>
     </row>
     <row r="4252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4252" s="1" t="s">
-        <v>4249</v>
+        <v>4250</v>
       </c>
       <c r="B4252" s="1" t="s">
-        <v>4249</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="4253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4253" s="1" t="s">
-        <v>4250</v>
+        <v>4251</v>
       </c>
       <c r="B4253" s="1" t="s">
-        <v>4250</v>
+        <v>4251</v>
       </c>
     </row>
     <row r="4254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4254" s="1" t="s">
-        <v>4251</v>
+        <v>4252</v>
       </c>
       <c r="B4254" s="1" t="s">
-        <v>4251</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="4255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4255" s="1" t="s">
-        <v>4252</v>
+        <v>4253</v>
       </c>
       <c r="B4255" s="1" t="s">
-        <v>4252</v>
+        <v>4253</v>
       </c>
     </row>
     <row r="4256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4256" s="1" t="s">
-        <v>4253</v>
+        <v>4254</v>
       </c>
       <c r="B4256" s="1" t="s">
-        <v>4253</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="4257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4257" s="1" t="s">
-        <v>4254</v>
+        <v>4255</v>
       </c>
       <c r="B4257" s="1" t="s">
-        <v>4254</v>
+        <v>4255</v>
       </c>
     </row>
     <row r="4258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4258" s="1" t="s">
-        <v>4255</v>
+        <v>4256</v>
       </c>
       <c r="B4258" s="1" t="s">
-        <v>4255</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="4259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4259" s="1" t="s">
-        <v>4256</v>
+        <v>4257</v>
       </c>
       <c r="B4259" s="1" t="s">
-        <v>4256</v>
+        <v>4257</v>
       </c>
     </row>
     <row r="4260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4260" s="1" t="s">
-        <v>4257</v>
+        <v>4258</v>
       </c>
       <c r="B4260" s="1" t="s">
-        <v>4257</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="4261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4261" s="1" t="s">
-        <v>4258</v>
+        <v>4259</v>
       </c>
       <c r="B4261" s="1" t="s">
-        <v>4258</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="4262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4262" s="1" t="s">
-        <v>4259</v>
+        <v>4260</v>
       </c>
       <c r="B4262" s="1" t="s">
-        <v>4259</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="4263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4263" s="1" t="s">
-        <v>4260</v>
+        <v>4261</v>
       </c>
       <c r="B4263" s="1" t="s">
-        <v>4260</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="4264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4264" s="1" t="s">
-        <v>4261</v>
+        <v>4262</v>
       </c>
       <c r="B4264" s="1" t="s">
-        <v>4261</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="4265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4265" s="1" t="s">
-        <v>4262</v>
+        <v>4263</v>
       </c>
       <c r="B4265" s="1" t="s">
-        <v>4262</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="4266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4266" s="1" t="s">
-        <v>4263</v>
+        <v>4264</v>
       </c>
       <c r="B4266" s="1" t="s">
-        <v>4263</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="4267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4267" s="1" t="s">
-        <v>4264</v>
+        <v>4265</v>
       </c>
       <c r="B4267" s="1" t="s">
-        <v>4264</v>
+        <v>4265</v>
       </c>
     </row>
     <row r="4268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4268" s="1" t="s">
-        <v>4265</v>
+        <v>4266</v>
       </c>
       <c r="B4268" s="1" t="s">
-        <v>4265</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="4269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4269" s="1" t="s">
-        <v>4266</v>
+        <v>4267</v>
       </c>
       <c r="B4269" s="1" t="s">
-        <v>4266</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="4270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4270" s="1" t="s">
-        <v>4267</v>
+        <v>4268</v>
       </c>
       <c r="B4270" s="1" t="s">
-        <v>4267</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="4271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4271" s="1" t="s">
-        <v>4268</v>
+        <v>4269</v>
       </c>
       <c r="B4271" s="1" t="s">
-        <v>4268</v>
+        <v>4269</v>
       </c>
     </row>
     <row r="4272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4272" s="1" t="s">
-        <v>4269</v>
+        <v>4270</v>
       </c>
       <c r="B4272" s="1" t="s">
-        <v>4269</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="4273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4273" s="1" t="s">
-        <v>4270</v>
+        <v>4271</v>
       </c>
       <c r="B4273" s="1" t="s">
-        <v>4447</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="4274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4274" s="1" t="s">
-        <v>4271</v>
+        <v>4272</v>
       </c>
       <c r="B4274" s="1" t="s">
-        <v>4409</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="4275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4275" s="1" t="s">
-        <v>4272</v>
+        <v>4273</v>
       </c>
       <c r="B4275" s="1" t="s">
-        <v>4272</v>
-      </c>
-    </row>
-    <row r="4276" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="4276" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4276" s="1" t="s">
-        <v>4273</v>
+        <v>4274</v>
       </c>
       <c r="B4276" s="1" t="s">
-        <v>4273</v>
-      </c>
-    </row>
-    <row r="4277" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="4277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4277" s="1" t="s">
-        <v>4274</v>
+        <v>4275</v>
       </c>
       <c r="B4277" s="1" t="s">
-        <v>4466</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="4278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4278" s="1" t="s">
-        <v>4275</v>
+        <v>4276</v>
       </c>
       <c r="B4278" s="1" t="s">
-        <v>4275</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="4279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4279" s="1" t="s">
-        <v>4276</v>
+        <v>4277</v>
       </c>
       <c r="B4279" s="1" t="s">
-        <v>4276</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="4280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4280" s="1" t="s">
-        <v>4277</v>
+        <v>4278</v>
       </c>
       <c r="B4280" s="1" t="s">
-        <v>4277</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="4281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4281" s="1" t="s">
-        <v>4278</v>
+        <v>4279</v>
       </c>
       <c r="B4281" s="1" t="s">
-        <v>4278</v>
+        <v>4279</v>
       </c>
     </row>
     <row r="4282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4282" s="1" t="s">
-        <v>4279</v>
+        <v>4280</v>
       </c>
       <c r="B4282" s="1" t="s">
-        <v>4279</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="4283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4283" s="1" t="s">
-        <v>4280</v>
+        <v>4281</v>
       </c>
       <c r="B4283" s="1" t="s">
-        <v>4280</v>
+        <v>4281</v>
       </c>
     </row>
     <row r="4284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4284" s="1" t="s">
-        <v>4281</v>
+        <v>4282</v>
       </c>
       <c r="B4284" s="1" t="s">
-        <v>4281</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="4285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4285" s="1" t="s">
-        <v>4282</v>
+        <v>4283</v>
       </c>
       <c r="B4285" s="1" t="s">
-        <v>4405</v>
+        <v>4283</v>
       </c>
     </row>
     <row r="4286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4286" s="1" t="s">
-        <v>4283</v>
+        <v>4284</v>
       </c>
       <c r="B4286" s="1" t="s">
-        <v>4283</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="4287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4287" s="1" t="s">
-        <v>4284</v>
+        <v>4285</v>
       </c>
       <c r="B4287" s="1" t="s">
-        <v>4284</v>
+        <v>4285</v>
       </c>
     </row>
     <row r="4288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4288" s="1" t="s">
-        <v>4285</v>
+        <v>4286</v>
       </c>
       <c r="B4288" s="1" t="s">
-        <v>4285</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="4289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4289" s="1" t="s">
-        <v>4286</v>
+        <v>4287</v>
       </c>
       <c r="B4289" s="1" t="s">
-        <v>4286</v>
+        <v>4287</v>
       </c>
     </row>
     <row r="4290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4290" s="1" t="s">
-        <v>4287</v>
+        <v>4288</v>
       </c>
       <c r="B4290" s="1" t="s">
-        <v>4287</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="4291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4291" s="1" t="s">
-        <v>4288</v>
+        <v>4289</v>
       </c>
       <c r="B4291" s="1" t="s">
-        <v>4288</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="4292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4292" s="1" t="s">
-        <v>4289</v>
+        <v>4290</v>
       </c>
       <c r="B4292" s="1" t="s">
-        <v>4289</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="4293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4293" s="1" t="s">
-        <v>4290</v>
+        <v>4291</v>
       </c>
       <c r="B4293" s="1" t="s">
-        <v>4290</v>
+        <v>4291</v>
       </c>
     </row>
     <row r="4294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4294" s="1" t="s">
-        <v>4291</v>
+        <v>4292</v>
       </c>
       <c r="B4294" s="1" t="s">
-        <v>4291</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="4295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4295" s="1" t="s">
-        <v>4292</v>
+        <v>4293</v>
       </c>
       <c r="B4295" s="1" t="s">
-        <v>4292</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="4296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4296" s="1" t="s">
-        <v>4293</v>
+        <v>4294</v>
       </c>
       <c r="B4296" s="1" t="s">
-        <v>4293</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="4297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4297" s="1" t="s">
-        <v>4294</v>
+        <v>4295</v>
       </c>
       <c r="B4297" s="1" t="s">
-        <v>4294</v>
+        <v>4295</v>
       </c>
     </row>
     <row r="4298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4298" s="1" t="s">
-        <v>4295</v>
+        <v>4296</v>
       </c>
       <c r="B4298" s="1" t="s">
-        <v>4295</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="4299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4299" s="1" t="s">
-        <v>4296</v>
+        <v>4297</v>
       </c>
       <c r="B4299" s="1" t="s">
-        <v>4296</v>
+        <v>4297</v>
       </c>
     </row>
     <row r="4300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4300" s="1" t="s">
-        <v>4297</v>
+        <v>4298</v>
       </c>
       <c r="B4300" s="1" t="s">
-        <v>4297</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="4301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4301" s="1" t="s">
-        <v>4298</v>
+        <v>4299</v>
       </c>
       <c r="B4301" s="1" t="s">
-        <v>4298</v>
+        <v>4299</v>
       </c>
     </row>
     <row r="4302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4302" s="1" t="s">
-        <v>4299</v>
+        <v>4406</v>
       </c>
       <c r="B4302" s="1" t="s">
-        <v>4299</v>
+        <v>4406</v>
       </c>
     </row>
     <row r="4303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4303" s="1" t="s">
-        <v>4406</v>
+        <v>4300</v>
       </c>
       <c r="B4303" s="1" t="s">
-        <v>4406</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="4304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4304" s="1" t="s">
-        <v>4300</v>
+        <v>4301</v>
       </c>
       <c r="B4304" s="1" t="s">
-        <v>4300</v>
+        <v>4301</v>
       </c>
     </row>
     <row r="4305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4305" s="1" t="s">
-        <v>4301</v>
+        <v>4302</v>
       </c>
       <c r="B4305" s="1" t="s">
-        <v>4301</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="4306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4306" s="1" t="s">
-        <v>4302</v>
+        <v>4303</v>
       </c>
       <c r="B4306" s="1" t="s">
-        <v>4302</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="4307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4307" s="1" t="s">
-        <v>4303</v>
+        <v>4304</v>
       </c>
       <c r="B4307" s="1" t="s">
-        <v>4303</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="4308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4308" s="1" t="s">
-        <v>4304</v>
+        <v>4305</v>
       </c>
       <c r="B4308" s="1" t="s">
-        <v>4304</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="4309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4309" s="1" t="s">
-        <v>4305</v>
+        <v>4306</v>
       </c>
       <c r="B4309" s="1" t="s">
-        <v>4305</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="4310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4310" s="1" t="s">
-        <v>4306</v>
+        <v>4307</v>
       </c>
       <c r="B4310" s="1" t="s">
-        <v>4306</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="4311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4311" s="1" t="s">
-        <v>4307</v>
+        <v>4308</v>
       </c>
       <c r="B4311" s="1" t="s">
-        <v>4307</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="4312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4312" s="1" t="s">
-        <v>4308</v>
+        <v>4309</v>
       </c>
       <c r="B4312" s="1" t="s">
-        <v>4308</v>
+        <v>4309</v>
       </c>
     </row>
     <row r="4313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4313" s="1" t="s">
-        <v>4309</v>
+        <v>4310</v>
       </c>
       <c r="B4313" s="1" t="s">
-        <v>4309</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="4314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4314" s="1" t="s">
-        <v>4310</v>
+        <v>4311</v>
       </c>
       <c r="B4314" s="1" t="s">
-        <v>4310</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="4315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4315" s="1" t="s">
-        <v>4311</v>
+        <v>4312</v>
       </c>
       <c r="B4315" s="1" t="s">
-        <v>4311</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="4316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4316" s="1" t="s">
-        <v>4312</v>
+        <v>4313</v>
       </c>
       <c r="B4316" s="1" t="s">
-        <v>4312</v>
+        <v>4313</v>
       </c>
     </row>
     <row r="4317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4317" s="1" t="s">
-        <v>4313</v>
+        <v>4314</v>
       </c>
       <c r="B4317" s="1" t="s">
-        <v>4313</v>
+        <v>4314</v>
+      </c>
+    </row>
+    <row r="4318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4318" s="1" t="s">
+        <v>4315</v>
+      </c>
+      <c r="B4318" s="1" t="s">
+        <v>4315</v>
       </c>
     </row>
     <row r="4319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4319" s="1" t="s">
-        <v>4314</v>
+        <v>4316</v>
       </c>
       <c r="B4319" s="1" t="s">
-        <v>4314</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="4320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4320" s="1" t="s">
-        <v>4315</v>
+        <v>4317</v>
       </c>
       <c r="B4320" s="1" t="s">
-        <v>4315</v>
+        <v>4317</v>
       </c>
     </row>
     <row r="4321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4321" s="1" t="s">
-        <v>4316</v>
+        <v>4318</v>
       </c>
       <c r="B4321" s="1" t="s">
-        <v>4316</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="4322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4322" s="1" t="s">
-        <v>4317</v>
+        <v>4319</v>
       </c>
       <c r="B4322" s="1" t="s">
-        <v>4317</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="4323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4323" s="1" t="s">
-        <v>4318</v>
+        <v>4320</v>
       </c>
       <c r="B4323" s="1" t="s">
-        <v>4318</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="4324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4324" s="1" t="s">
-        <v>4319</v>
+        <v>4321</v>
       </c>
       <c r="B4324" s="1" t="s">
-        <v>4319</v>
+        <v>4321</v>
       </c>
     </row>
     <row r="4325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4325" s="1" t="s">
-        <v>4320</v>
+        <v>4322</v>
       </c>
       <c r="B4325" s="1" t="s">
-        <v>4320</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="4326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4326" s="1" t="s">
-        <v>4321</v>
+        <v>4323</v>
       </c>
       <c r="B4326" s="1" t="s">
-        <v>4321</v>
+        <v>4323</v>
       </c>
     </row>
     <row r="4327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4327" s="1" t="s">
-        <v>4322</v>
+        <v>4324</v>
       </c>
       <c r="B4327" s="1" t="s">
-        <v>4322</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="4328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4328" s="1" t="s">
-        <v>4323</v>
+        <v>4325</v>
       </c>
       <c r="B4328" s="1" t="s">
-        <v>4323</v>
+        <v>4325</v>
       </c>
     </row>
     <row r="4329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4329" s="1" t="s">
-        <v>4324</v>
+        <v>4326</v>
       </c>
       <c r="B4329" s="1" t="s">
-        <v>4324</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="4330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4330" s="1" t="s">
-        <v>4325</v>
+        <v>4327</v>
       </c>
       <c r="B4330" s="1" t="s">
-        <v>4325</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="4331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4331" s="1" t="s">
-        <v>4326</v>
+        <v>4328</v>
       </c>
       <c r="B4331" s="1" t="s">
-        <v>4326</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="4332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4332" s="1" t="s">
-        <v>4327</v>
+        <v>4329</v>
       </c>
       <c r="B4332" s="1" t="s">
-        <v>4327</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="4333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4333" s="1" t="s">
-        <v>4328</v>
+        <v>4330</v>
       </c>
       <c r="B4333" s="1" t="s">
-        <v>4328</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="4334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4334" s="1" t="s">
-        <v>4329</v>
+        <v>4331</v>
       </c>
       <c r="B4334" s="1" t="s">
-        <v>4329</v>
+        <v>4331</v>
       </c>
     </row>
     <row r="4335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4335" s="1" t="s">
-        <v>4330</v>
+        <v>4332</v>
       </c>
       <c r="B4335" s="1" t="s">
-        <v>4330</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="4336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4336" s="1" t="s">
-        <v>4331</v>
+        <v>4333</v>
       </c>
       <c r="B4336" s="1" t="s">
-        <v>4331</v>
+        <v>4333</v>
       </c>
     </row>
     <row r="4337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4337" s="1" t="s">
-        <v>4332</v>
+        <v>4334</v>
       </c>
       <c r="B4337" s="1" t="s">
-        <v>4332</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="4338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4338" s="1" t="s">
-        <v>4333</v>
+        <v>4335</v>
       </c>
       <c r="B4338" s="1" t="s">
-        <v>4333</v>
+        <v>4335</v>
       </c>
     </row>
     <row r="4339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4339" s="1" t="s">
-        <v>4334</v>
+        <v>4336</v>
       </c>
       <c r="B4339" s="1" t="s">
-        <v>4334</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="4340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4340" s="1" t="s">
-        <v>4335</v>
+        <v>4337</v>
       </c>
       <c r="B4340" s="1" t="s">
-        <v>4335</v>
+        <v>4337</v>
       </c>
     </row>
     <row r="4341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4341" s="1" t="s">
-        <v>4336</v>
+        <v>4338</v>
       </c>
       <c r="B4341" s="1" t="s">
-        <v>4336</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="4342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4342" s="1" t="s">
-        <v>4337</v>
+        <v>4339</v>
       </c>
       <c r="B4342" s="1" t="s">
-        <v>4337</v>
+        <v>4339</v>
       </c>
     </row>
     <row r="4343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4343" s="1" t="s">
-        <v>4338</v>
+        <v>4340</v>
       </c>
       <c r="B4343" s="1" t="s">
-        <v>4338</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="4344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4344" s="1" t="s">
-        <v>4339</v>
+        <v>4341</v>
       </c>
       <c r="B4344" s="1" t="s">
-        <v>4339</v>
+        <v>4341</v>
       </c>
     </row>
     <row r="4345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4345" s="1" t="s">
-        <v>4340</v>
+        <v>4342</v>
       </c>
       <c r="B4345" s="1" t="s">
-        <v>4340</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="4346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4346" s="1" t="s">
-        <v>4341</v>
+        <v>4343</v>
       </c>
       <c r="B4346" s="1" t="s">
-        <v>4341</v>
+        <v>4343</v>
       </c>
     </row>
     <row r="4347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4347" s="1" t="s">
-        <v>4342</v>
+        <v>4344</v>
       </c>
       <c r="B4347" s="1" t="s">
-        <v>4342</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="4348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4348" s="1" t="s">
-        <v>4343</v>
+        <v>4345</v>
       </c>
       <c r="B4348" s="1" t="s">
-        <v>4343</v>
+        <v>4345</v>
       </c>
     </row>
     <row r="4349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4349" s="1" t="s">
-        <v>4344</v>
+        <v>4346</v>
       </c>
       <c r="B4349" s="1" t="s">
-        <v>4344</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="4350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4350" s="1" t="s">
-        <v>4345</v>
+        <v>4347</v>
       </c>
       <c r="B4350" s="1" t="s">
-        <v>4345</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="4351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4351" s="1" t="s">
-        <v>4346</v>
+        <v>4348</v>
       </c>
       <c r="B4351" s="1" t="s">
-        <v>4346</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="4352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4352" s="1" t="s">
-        <v>4347</v>
+        <v>4349</v>
       </c>
       <c r="B4352" s="1" t="s">
-        <v>4347</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="4353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4353" s="1" t="s">
-        <v>4348</v>
+        <v>4350</v>
       </c>
       <c r="B4353" s="1" t="s">
-        <v>4348</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="4354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4354" s="1" t="s">
-        <v>4349</v>
+        <v>4351</v>
       </c>
       <c r="B4354" s="1" t="s">
-        <v>4349</v>
+        <v>4351</v>
       </c>
     </row>
     <row r="4355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4355" s="1" t="s">
-        <v>4350</v>
+        <v>4352</v>
       </c>
       <c r="B4355" s="1" t="s">
-        <v>4350</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="4356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4356" s="1" t="s">
-        <v>4351</v>
+        <v>4353</v>
       </c>
       <c r="B4356" s="1" t="s">
-        <v>4351</v>
+        <v>4353</v>
       </c>
     </row>
     <row r="4357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4357" s="1" t="s">
-        <v>4352</v>
+        <v>4354</v>
       </c>
       <c r="B4357" s="1" t="s">
-        <v>4352</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="4358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4358" s="1" t="s">
-        <v>4353</v>
+        <v>4355</v>
       </c>
       <c r="B4358" s="1" t="s">
-        <v>4353</v>
+        <v>4355</v>
       </c>
     </row>
     <row r="4359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4359" s="1" t="s">
-        <v>4354</v>
+        <v>4356</v>
       </c>
       <c r="B4359" s="1" t="s">
-        <v>4354</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="4360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4360" s="1" t="s">
-        <v>4355</v>
+        <v>4357</v>
       </c>
       <c r="B4360" s="1" t="s">
-        <v>4355</v>
+        <v>4357</v>
       </c>
     </row>
     <row r="4361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4361" s="1" t="s">
-        <v>4356</v>
+        <v>4358</v>
       </c>
       <c r="B4361" s="1" t="s">
-        <v>4356</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="4362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4362" s="1" t="s">
-        <v>4357</v>
+        <v>4359</v>
       </c>
       <c r="B4362" s="1" t="s">
-        <v>4357</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="4363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4363" s="1" t="s">
-        <v>4358</v>
+        <v>4360</v>
       </c>
       <c r="B4363" s="1" t="s">
-        <v>4358</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="4364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4364" s="1" t="s">
-        <v>4359</v>
+        <v>4361</v>
       </c>
       <c r="B4364" s="1" t="s">
-        <v>4359</v>
+        <v>4361</v>
       </c>
     </row>
     <row r="4365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4365" s="1" t="s">
-        <v>4360</v>
+        <v>4362</v>
       </c>
       <c r="B4365" s="1" t="s">
-        <v>4360</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="4366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4366" s="1" t="s">
-        <v>4361</v>
+        <v>4363</v>
       </c>
       <c r="B4366" s="1" t="s">
-        <v>4361</v>
+        <v>4363</v>
       </c>
     </row>
     <row r="4367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4367" s="1" t="s">
-        <v>4362</v>
+        <v>4364</v>
       </c>
       <c r="B4367" s="1" t="s">
-        <v>4362</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="4368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4368" s="1" t="s">
-        <v>4363</v>
+        <v>4365</v>
       </c>
       <c r="B4368" s="1" t="s">
-        <v>4363</v>
+        <v>4365</v>
       </c>
     </row>
     <row r="4369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4369" s="1" t="s">
-        <v>4364</v>
+        <v>4366</v>
       </c>
       <c r="B4369" s="1" t="s">
-        <v>4364</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="4370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4370" s="1" t="s">
-        <v>4365</v>
+        <v>4367</v>
       </c>
       <c r="B4370" s="1" t="s">
-        <v>4365</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="4371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4371" s="1" t="s">
-        <v>4366</v>
+        <v>4368</v>
       </c>
       <c r="B4371" s="1" t="s">
-        <v>4366</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="4372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4372" s="1" t="s">
-        <v>4367</v>
+        <v>4369</v>
       </c>
       <c r="B4372" s="1" t="s">
-        <v>4367</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="4373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4373" s="1" t="s">
-        <v>4368</v>
+        <v>4370</v>
       </c>
       <c r="B4373" s="1" t="s">
-        <v>4368</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="4374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4374" s="1" t="s">
-        <v>4369</v>
+        <v>4371</v>
       </c>
       <c r="B4374" s="1" t="s">
-        <v>4369</v>
+        <v>4371</v>
       </c>
     </row>
     <row r="4375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4375" s="1" t="s">
-        <v>4370</v>
+        <v>4372</v>
       </c>
       <c r="B4375" s="1" t="s">
-        <v>4370</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="4376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4376" s="1" t="s">
-        <v>4371</v>
+        <v>4373</v>
       </c>
       <c r="B4376" s="1" t="s">
-        <v>4371</v>
+        <v>4373</v>
       </c>
     </row>
     <row r="4377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4377" s="1" t="s">
-        <v>4372</v>
+        <v>4374</v>
       </c>
       <c r="B4377" s="1" t="s">
-        <v>4372</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="4378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4378" s="1" t="s">
-        <v>4373</v>
+        <v>4375</v>
       </c>
       <c r="B4378" s="1" t="s">
-        <v>4373</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="4379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4379" s="1" t="s">
-        <v>4374</v>
+        <v>4376</v>
       </c>
       <c r="B4379" s="1" t="s">
-        <v>4374</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="4380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4380" s="1" t="s">
-        <v>4375</v>
+        <v>4377</v>
       </c>
       <c r="B4380" s="1" t="s">
-        <v>4375</v>
+        <v>4377</v>
       </c>
     </row>
     <row r="4381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4381" s="1" t="s">
-        <v>4376</v>
+        <v>4378</v>
       </c>
       <c r="B4381" s="1" t="s">
-        <v>4376</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="4382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4382" s="1" t="s">
-        <v>4377</v>
+        <v>4379</v>
       </c>
       <c r="B4382" s="1" t="s">
-        <v>4377</v>
+        <v>4379</v>
       </c>
     </row>
     <row r="4383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4383" s="1" t="s">
-        <v>4378</v>
+        <v>4380</v>
       </c>
       <c r="B4383" s="1" t="s">
-        <v>4378</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="4384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4384" s="1" t="s">
-        <v>4379</v>
+        <v>4381</v>
       </c>
       <c r="B4384" s="1" t="s">
-        <v>4379</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="4385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4385" s="1" t="s">
-        <v>4380</v>
+        <v>4382</v>
       </c>
       <c r="B4385" s="1" t="s">
-        <v>4380</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="4386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4386" s="1" t="s">
-        <v>4381</v>
+        <v>4383</v>
       </c>
       <c r="B4386" s="1" t="s">
-        <v>4381</v>
+        <v>4383</v>
       </c>
     </row>
     <row r="4387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4387" s="1" t="s">
-        <v>4382</v>
+        <v>4384</v>
       </c>
       <c r="B4387" s="1" t="s">
-        <v>4382</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="4388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4388" s="1" t="s">
-        <v>4383</v>
+        <v>4385</v>
       </c>
       <c r="B4388" s="1" t="s">
-        <v>4383</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="4389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4389" s="1" t="s">
-        <v>4384</v>
+        <v>4386</v>
       </c>
       <c r="B4389" s="1" t="s">
-        <v>4384</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="4390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4390" s="1" t="s">
-        <v>4385</v>
+        <v>4387</v>
       </c>
       <c r="B4390" s="1" t="s">
-        <v>4385</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="4391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4391" s="1" t="s">
-        <v>4386</v>
+        <v>4388</v>
       </c>
       <c r="B4391" s="1" t="s">
-        <v>4386</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="4392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4392" s="1" t="s">
-        <v>4387</v>
+        <v>4389</v>
       </c>
       <c r="B4392" s="1" t="s">
-        <v>4387</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="4393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4393" s="1" t="s">
-        <v>4388</v>
+        <v>4390</v>
       </c>
       <c r="B4393" s="1" t="s">
-        <v>4388</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="4394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4394" s="1" t="s">
-        <v>4389</v>
+        <v>4391</v>
       </c>
       <c r="B4394" s="1" t="s">
-        <v>4389</v>
+        <v>4391</v>
       </c>
     </row>
     <row r="4395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4395" s="1" t="s">
-        <v>4390</v>
+        <v>4392</v>
       </c>
       <c r="B4395" s="1" t="s">
-        <v>4390</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="4396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4396" s="1" t="s">
-        <v>4391</v>
+        <v>4393</v>
       </c>
       <c r="B4396" s="1" t="s">
-        <v>4391</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="4397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4397" s="1" t="s">
-        <v>4392</v>
+        <v>4394</v>
       </c>
       <c r="B4397" s="1" t="s">
-        <v>4392</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="4398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4398" s="1" t="s">
-        <v>4393</v>
+        <v>4395</v>
       </c>
       <c r="B4398" s="1" t="s">
-        <v>4393</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="4399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4399" s="1" t="s">
-        <v>4394</v>
+        <v>4396</v>
       </c>
       <c r="B4399" s="1" t="s">
-        <v>4394</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="4400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4400" s="1" t="s">
-        <v>4395</v>
+        <v>4397</v>
       </c>
       <c r="B4400" s="1" t="s">
-        <v>4395</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="4401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4401" s="1" t="s">
-        <v>4396</v>
+        <v>4398</v>
       </c>
       <c r="B4401" s="1" t="s">
-        <v>4396</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="4402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4402" s="1" t="s">
-        <v>4397</v>
+        <v>4399</v>
       </c>
       <c r="B4402" s="1" t="s">
-        <v>4397</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="4403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4403" s="1" t="s">
-        <v>4398</v>
+        <v>4400</v>
       </c>
       <c r="B4403" s="1" t="s">
-        <v>4398</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="4404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4404" s="1" t="s">
-        <v>4399</v>
+        <v>4401</v>
       </c>
       <c r="B4404" s="1" t="s">
-        <v>4399</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="4405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4405" s="1" t="s">
-        <v>4400</v>
+        <v>4402</v>
       </c>
       <c r="B4405" s="1" t="s">
-        <v>4400</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="4406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4406" s="1" t="s">
-        <v>4401</v>
+        <v>4403</v>
       </c>
       <c r="B4406" s="1" t="s">
-        <v>4401</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="4407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4407" s="1" t="s">
-        <v>4402</v>
+        <v>4404</v>
       </c>
       <c r="B4407" s="1" t="s">
-        <v>4402</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="4408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4408" s="1" t="s">
-        <v>4403</v>
+        <v>4407</v>
       </c>
       <c r="B4408" s="1" t="s">
-        <v>4403</v>
+        <v>4408</v>
       </c>
     </row>
     <row r="4409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4409" s="1" t="s">
-        <v>4404</v>
+        <v>4410</v>
       </c>
       <c r="B4409" s="1" t="s">
-        <v>4404</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="4410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4410" s="1" t="s">
-        <v>4407</v>
-      </c>
-      <c r="B4410" s="1" t="s">
-        <v>4408</v>
+        <v>4411</v>
+      </c>
+      <c r="B4410" t="s">
+        <v>4412</v>
       </c>
     </row>
     <row r="4411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4411" s="1" t="s">
-        <v>4410</v>
+        <v>4413</v>
       </c>
       <c r="B4411" s="1" t="s">
-        <v>4410</v>
+        <v>4414</v>
       </c>
     </row>
     <row r="4412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4412" s="1" t="s">
-        <v>4411</v>
-      </c>
-      <c r="B4412" t="s">
-        <v>4412</v>
+        <v>4415</v>
+      </c>
+      <c r="B4412" s="1" t="s">
+        <v>4414</v>
       </c>
     </row>
     <row r="4413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4413" s="1" t="s">
-        <v>4413</v>
+        <v>4416</v>
       </c>
       <c r="B4413" s="1" t="s">
-        <v>4414</v>
-      </c>
-    </row>
-    <row r="4414" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4416</v>
+      </c>
+    </row>
+    <row r="4414" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4414" s="1" t="s">
-        <v>4415</v>
+        <v>4417</v>
       </c>
       <c r="B4414" s="1" t="s">
-        <v>4414</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="4415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4415" s="1" t="s">
-        <v>4416</v>
+        <v>4419</v>
       </c>
       <c r="B4415" s="1" t="s">
-        <v>4416</v>
-      </c>
-    </row>
-    <row r="4416" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="4416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4416" s="1" t="s">
-        <v>4417</v>
+        <v>4420</v>
       </c>
       <c r="B4416" s="1" t="s">
-        <v>4418</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="4417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4417" s="1" t="s">
-        <v>4419</v>
+        <v>4422</v>
       </c>
       <c r="B4417" s="1" t="s">
-        <v>4419</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="4418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4418" s="1" t="s">
-        <v>4420</v>
+        <v>4424</v>
       </c>
       <c r="B4418" s="1" t="s">
-        <v>4421</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="4419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4419" s="1" t="s">
-        <v>4422</v>
+        <v>4426</v>
       </c>
       <c r="B4419" s="1" t="s">
-        <v>4423</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="4420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4420" s="1" t="s">
-        <v>4424</v>
+        <v>4427</v>
       </c>
       <c r="B4420" s="1" t="s">
-        <v>4425</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="4421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4421" s="1" t="s">
-        <v>4426</v>
+        <v>4429</v>
       </c>
       <c r="B4421" s="1" t="s">
-        <v>4426</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="4422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4422" s="1" t="s">
-        <v>4427</v>
+        <v>4430</v>
       </c>
       <c r="B4422" s="1" t="s">
-        <v>4428</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="4423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4423" s="1" t="s">
-        <v>4429</v>
+        <v>4432</v>
       </c>
       <c r="B4423" s="1" t="s">
-        <v>4429</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="4424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4424" s="1" t="s">
-        <v>4430</v>
+        <v>4433</v>
       </c>
       <c r="B4424" s="1" t="s">
-        <v>4431</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="4425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4425" s="1" t="s">
-        <v>4432</v>
+        <v>4434</v>
       </c>
       <c r="B4425" s="1" t="s">
-        <v>4432</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="4426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4426" s="1" t="s">
-        <v>4433</v>
+        <v>4435</v>
       </c>
       <c r="B4426" s="1" t="s">
-        <v>4433</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="4427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4427" s="1" t="s">
-        <v>4434</v>
+        <v>4437</v>
       </c>
       <c r="B4427" s="1" t="s">
-        <v>4436</v>
+        <v>4437</v>
       </c>
     </row>
     <row r="4428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4428" s="1" t="s">
-        <v>4435</v>
+        <v>4438</v>
       </c>
       <c r="B4428" s="1" t="s">
-        <v>4436</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="4429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4429" s="1" t="s">
-        <v>4437</v>
+        <v>4440</v>
       </c>
       <c r="B4429" s="1" t="s">
-        <v>4437</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="4430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4430" s="1" t="s">
-        <v>4438</v>
+        <v>4441</v>
       </c>
       <c r="B4430" s="1" t="s">
         <v>4439</v>
@@ -49427,147 +49998,841 @@
     </row>
     <row r="4431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4431" s="1" t="s">
-        <v>4440</v>
+        <v>3742</v>
       </c>
       <c r="B4431" s="1" t="s">
-        <v>4440</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="4432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4432" s="1" t="s">
-        <v>4441</v>
+        <v>4444</v>
       </c>
       <c r="B4432" s="1" t="s">
-        <v>4439</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="4433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4433" s="1" t="s">
-        <v>3742</v>
+        <v>4445</v>
       </c>
       <c r="B4433" s="1" t="s">
-        <v>4442</v>
-      </c>
-    </row>
-    <row r="4434" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4446</v>
+      </c>
+    </row>
+    <row r="4434" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4434" s="1" t="s">
-        <v>4444</v>
+        <v>4452</v>
       </c>
       <c r="B4434" s="1" t="s">
-        <v>4444</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="4435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4435" s="1" t="s">
-        <v>4445</v>
+        <v>4453</v>
       </c>
       <c r="B4435" s="1" t="s">
-        <v>4446</v>
-      </c>
-    </row>
-    <row r="4436" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="4436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4436" s="1" t="s">
-        <v>4452</v>
+        <v>4458</v>
       </c>
       <c r="B4436" s="1" t="s">
-        <v>4455</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="4437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4437" s="1" t="s">
-        <v>4453</v>
+        <v>4462</v>
       </c>
       <c r="B4437" s="1" t="s">
-        <v>4454</v>
-      </c>
-    </row>
-    <row r="4438" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="4438" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4438" s="1" t="s">
-        <v>4458</v>
+        <v>4467</v>
       </c>
       <c r="B4438" s="1" t="s">
-        <v>4457</v>
-      </c>
-    </row>
-    <row r="4439" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="4439" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4439" s="1" t="s">
-        <v>4462</v>
+        <v>4469</v>
       </c>
       <c r="B4439" s="1" t="s">
-        <v>4461</v>
-      </c>
-    </row>
-    <row r="4440" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="4440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4440" s="1" t="s">
-        <v>4467</v>
+        <v>4471</v>
       </c>
       <c r="B4440" s="1" t="s">
-        <v>4466</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="4441" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4441" s="1" t="s">
-        <v>4469</v>
+        <v>4473</v>
       </c>
       <c r="B4441" s="1" t="s">
-        <v>4468</v>
+        <v>4474</v>
+      </c>
+    </row>
+    <row r="4442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4442" s="1" t="s">
+        <v>4475</v>
+      </c>
+      <c r="B4442" s="1" t="s">
+        <v>4477</v>
+      </c>
+    </row>
+    <row r="4443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4443" s="1" t="s">
+        <v>4476</v>
+      </c>
+      <c r="B4443" s="1" t="s">
+        <v>4478</v>
+      </c>
+    </row>
+    <row r="4444" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4444" s="1" t="s">
+        <v>4479</v>
+      </c>
+      <c r="B4444" s="1" t="s">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="4445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4445" s="1" t="s">
+        <v>4481</v>
+      </c>
+      <c r="B4445" s="1" t="s">
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="4446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4446" s="1" t="s">
+        <v>4482</v>
+      </c>
+      <c r="B4446" s="1" t="s">
+        <v>4484</v>
+      </c>
+    </row>
+    <row r="4447" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4447" s="1" t="s">
+        <v>4485</v>
+      </c>
+      <c r="B4447" s="1" t="s">
+        <v>4486</v>
+      </c>
+    </row>
+    <row r="4448" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4448" s="1" t="s">
+        <v>4488</v>
+      </c>
+      <c r="B4448" s="1" t="s">
+        <v>4489</v>
+      </c>
+    </row>
+    <row r="4449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4449" s="1" t="s">
+        <v>4490</v>
+      </c>
+      <c r="B4449" s="1" t="s">
+        <v>4491</v>
+      </c>
+    </row>
+    <row r="4450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4450" s="1" t="s">
+        <v>4492</v>
+      </c>
+      <c r="B4450" s="1" t="s">
+        <v>4493</v>
+      </c>
+    </row>
+    <row r="4451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4451" s="1" t="s">
+        <v>4494</v>
+      </c>
+      <c r="B4451" s="1" t="s">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="4452" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4452" s="1" t="s">
+        <v>4496</v>
+      </c>
+      <c r="B4452" s="1" t="s">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="4453" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4453" s="1" t="s">
+        <v>4505</v>
+      </c>
+      <c r="B4453" s="1" t="s">
+        <v>4506</v>
+      </c>
+    </row>
+    <row r="4454" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4454" s="1" t="s">
+        <v>4508</v>
+      </c>
+      <c r="B4454" s="1" t="s">
+        <v>4509</v>
+      </c>
+    </row>
+    <row r="4455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4455" s="1" t="s">
+        <v>4511</v>
+      </c>
+      <c r="B4455" s="1" t="s">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="4456" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4456" s="1" t="s">
+        <v>4513</v>
+      </c>
+      <c r="B4456" s="1" t="s">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="4457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4457" s="1" t="s">
+        <v>4514</v>
+      </c>
+      <c r="B4457" s="1" t="s">
+        <v>4517</v>
+      </c>
+    </row>
+    <row r="4458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4458" s="1" t="s">
+        <v>4515</v>
+      </c>
+      <c r="B4458" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4459" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4459" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B4459" s="1" t="s">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="4460" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4460" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B4460" s="1" t="s">
+        <v>4522</v>
+      </c>
+    </row>
+    <row r="4461" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4461" s="1" t="s">
+        <v>4523</v>
+      </c>
+      <c r="B4461" s="1" t="s">
+        <v>4524</v>
+      </c>
+    </row>
+    <row r="4462" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4462" s="1" t="s">
+        <v>4529</v>
+      </c>
+      <c r="B4462" s="1" t="s">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="4463" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4463" s="1" t="s">
+        <v>4530</v>
+      </c>
+      <c r="B4463" s="1" t="s">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="4464" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4464" s="1" t="s">
+        <v>4535</v>
+      </c>
+      <c r="B4464" s="1" t="s">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="4465" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4465" s="1" t="s">
+        <v>4536</v>
+      </c>
+      <c r="B4465" s="1" t="s">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="4466" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4466" s="1" t="s">
+        <v>4539</v>
+      </c>
+      <c r="B4466" s="1" t="s">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="4467" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4467" s="1" t="s">
+        <v>4540</v>
+      </c>
+      <c r="B4467" s="1" t="s">
+        <v>4542</v>
+      </c>
+    </row>
+    <row r="4468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4468" s="1" t="s">
+        <v>4543</v>
+      </c>
+      <c r="B4468" s="1" t="s">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="4469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4469" s="1" t="s">
+        <v>4544</v>
+      </c>
+      <c r="B4469" s="1" t="s">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="4470" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4470" s="1" t="s">
+        <v>4545</v>
+      </c>
+      <c r="B4470" s="1" t="s">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="4471" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4471" s="1" t="s">
+        <v>4546</v>
+      </c>
+      <c r="B4471" s="1" t="s">
+        <v>4549</v>
+      </c>
+    </row>
+    <row r="4472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4472" s="1" t="s">
+        <v>4553</v>
+      </c>
+      <c r="B4472" s="1" t="s">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="4473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4473" s="1" t="s">
+        <v>4554</v>
+      </c>
+      <c r="B4473" s="1" t="s">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="4474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4474" s="1" t="s">
+        <v>4555</v>
+      </c>
+      <c r="B4474" s="1" t="s">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="4475" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4475" s="1" t="s">
+        <v>4556</v>
+      </c>
+      <c r="B4475" s="1" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="4476" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4476" s="1" t="s">
+        <v>4557</v>
+      </c>
+      <c r="B4476" s="1" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="4477" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4477" s="1" t="s">
+        <v>4558</v>
+      </c>
+      <c r="B4477" s="1" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="4478" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4478" s="1" t="s">
+        <v>4561</v>
+      </c>
+      <c r="B4478" s="1" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4479" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4479" s="1" t="s">
+        <v>4562</v>
+      </c>
+      <c r="B4479" s="1" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4480" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4480" s="1" t="s">
+        <v>4563</v>
+      </c>
+      <c r="B4480" s="1" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4481" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4481" s="1" t="s">
+        <v>4564</v>
+      </c>
+      <c r="B4481" s="1" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="4482" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4482" s="1" t="s">
+        <v>4565</v>
+      </c>
+      <c r="B4482" s="1" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="4483" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4483" s="1" t="s">
+        <v>4566</v>
+      </c>
+      <c r="B4483" s="1" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="4484" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4484" s="1" t="s">
+        <v>4568</v>
+      </c>
+      <c r="B4484" s="1" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4485" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4485" s="1" t="s">
+        <v>4569</v>
+      </c>
+      <c r="B4485" s="1" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="4486" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4486" s="1" t="s">
+        <v>4573</v>
+      </c>
+      <c r="B4486" s="1" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="4487" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4487" s="1" t="s">
+        <v>4574</v>
+      </c>
+      <c r="B4487" s="1" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="4488" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4488" s="1" t="s">
+        <v>4575</v>
+      </c>
+      <c r="B4488" s="1" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="4489" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4489" s="1" t="s">
+        <v>4576</v>
+      </c>
+      <c r="B4489" s="1" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="4490" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4490" s="1" t="s">
+        <v>4579</v>
+      </c>
+      <c r="B4490" s="1" t="s">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="4491" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4491" s="1" t="s">
+        <v>4580</v>
+      </c>
+      <c r="B4491" s="1" t="s">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="4492" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4492" s="1" t="s">
+        <v>4581</v>
+      </c>
+      <c r="B4492" s="1" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4493" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4493" s="1" t="s">
+        <v>4582</v>
+      </c>
+      <c r="B4493" s="1" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4494" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4494" s="1" t="s">
+        <v>4585</v>
+      </c>
+      <c r="B4494" s="1" t="s">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="4495" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4495" s="1" t="s">
+        <v>4586</v>
+      </c>
+      <c r="B4495" s="1" t="s">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="4496" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4496" s="1" t="s">
+        <v>4587</v>
+      </c>
+      <c r="B4496" s="1" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4497" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4497" s="1" t="s">
+        <v>4588</v>
+      </c>
+      <c r="B4497" s="1" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4498" s="1" t="s">
+        <v>4592</v>
+      </c>
+      <c r="B4498" s="1" t="s">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="4499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4499" s="1" t="s">
+        <v>4591</v>
+      </c>
+      <c r="B4499" s="1" t="s">
+        <v>4594</v>
+      </c>
+    </row>
+    <row r="4500" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4500" s="1" t="s">
+        <v>4595</v>
+      </c>
+      <c r="B4500" s="1" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4501" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4501" s="1" t="s">
+        <v>4596</v>
+      </c>
+      <c r="B4501" s="1" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4502" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4502" s="1" t="s">
+        <v>4597</v>
+      </c>
+      <c r="B4502" s="1" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4503" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4503" s="1" t="s">
+        <v>4598</v>
+      </c>
+      <c r="B4503" s="1" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4504" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4504" s="1" t="s">
+        <v>4600</v>
+      </c>
+      <c r="B4504" s="1" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4505" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4505" s="1" t="s">
+        <v>4601</v>
+      </c>
+      <c r="B4505" s="1" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4506" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4506" s="1" t="s">
+        <v>4602</v>
+      </c>
+      <c r="B4506" s="1" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4507" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4507" s="1" t="s">
+        <v>4603</v>
+      </c>
+      <c r="B4507" s="1" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4508" s="1" t="s">
+        <v>4606</v>
+      </c>
+      <c r="B4508" s="1" t="s">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="4509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4509" s="1" t="s">
+        <v>4607</v>
+      </c>
+      <c r="B4509" s="1" t="s">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="4510" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4510" s="1" t="s">
+        <v>4615</v>
+      </c>
+      <c r="B4510" s="1" t="s">
+        <v>4617</v>
+      </c>
+    </row>
+    <row r="4511" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4511" s="1" t="s">
+        <v>4616</v>
+      </c>
+      <c r="B4511" s="1" t="s">
+        <v>4617</v>
+      </c>
+    </row>
+    <row r="4512" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4512" s="1" t="s">
+        <v>4619</v>
+      </c>
+      <c r="B4512" s="1" t="s">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="4513" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4513" s="1" t="s">
+        <v>4621</v>
+      </c>
+      <c r="B4513" s="1" t="s">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="4514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4514" s="1" t="s">
+        <v>4623</v>
+      </c>
+      <c r="B4514" s="1" t="s">
+        <v>4626</v>
+      </c>
+    </row>
+    <row r="4515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4515" s="1" t="s">
+        <v>4624</v>
+      </c>
+      <c r="B4515" s="1" t="s">
+        <v>4625</v>
+      </c>
+    </row>
+    <row r="4516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4516" s="1" t="s">
+        <v>4628</v>
+      </c>
+      <c r="B4516" s="1" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="4517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4517" s="1" t="s">
+        <v>4629</v>
+      </c>
+      <c r="B4517" s="1" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="4518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4518" s="1" t="s">
+        <v>4630</v>
+      </c>
+      <c r="B4518" s="1" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="4519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4519" s="1" t="s">
+        <v>4631</v>
+      </c>
+      <c r="B4519" s="1" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="4520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4520" s="1" t="s">
+        <v>4635</v>
+      </c>
+      <c r="B4520" s="1" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="4521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4521" s="1" t="s">
+        <v>4636</v>
+      </c>
+      <c r="B4521" s="1" t="s">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="4522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4522" s="1" t="s">
+        <v>4637</v>
+      </c>
+      <c r="B4522" s="1" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="4523" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4523" s="1" t="s">
+        <v>4638</v>
+      </c>
+      <c r="B4523" s="1" t="s">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="4524" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4524" s="1" t="s">
+        <v>4639</v>
+      </c>
+      <c r="B4524" s="1" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="4525" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4525" s="1" t="s">
+        <v>4640</v>
+      </c>
+      <c r="B4525" s="1" t="s">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="4526" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4526" s="1" t="s">
+        <v>4641</v>
+      </c>
+      <c r="B4526" s="1" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="4527" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4527" s="1" t="s">
+        <v>4642</v>
+      </c>
+      <c r="B4527" s="1" t="s">
+        <v>4644</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="23" priority="94"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="21" priority="64"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="19" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="17" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="65"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3831 A3894:A4189 A6734:A1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="103"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="105"/>
+  <conditionalFormatting sqref="A6732:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3831 A3894:A4189">
+    <cfRule type="duplicateValues" dxfId="18" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="14" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3832:A3893">
-    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4412 A2044 A2035:B2043 A2034 A2045:B4411 A1:B2033 A4413:B1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+  <conditionalFormatting sqref="A4410 A2044 A2035:B2043 A2034 A4411:B4460 A4461:A4462 A4463:B4499 B4500:B4503 A1:B2033 A2045:B4409 A4504:B1048576">
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B209:B1631 B1:B23 B25:B84 B143 B1805:B1809 B3442:B3831 B3894:B4189 B6734:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
+  <conditionalFormatting sqref="B6732:B1048576 B1:B23 B25:B84 B143 B1805:B1809 B3442:B3831 B3894:B4189 B209:B1631">
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B2033 B2045:B3339 B2035:B2043">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  <conditionalFormatting sqref="B1810:B2033 B2035:B2043 B2045:B3339">
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3832:B3893">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3206">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1556">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
xóa thừa ở mệnh
</commit_message>
<xml_diff>
--- a/LuanPhuThe.xlsx
+++ b/LuanPhuThe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FED248-0F5E-4A22-A015-59CF26DB1399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFB720C-3731-48E2-9163-B207670E461F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9042" uniqueCount="4699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9046" uniqueCount="4703">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -14129,6 +14129,18 @@
   </si>
   <si>
     <t>Người hôn phối là người hiền hậu, nhẹ nhàng, đức độ, sống tình nghĩa, nhường nhịn, lâu bền với nhau, ít khi xảy ra mâu thuẫn. Khi có mâu thuẫn thì hạ cái tôi của mình xuống ngay, để giảng hòa. Hai vợ chồng tường đối xứng đôi vừa lứa với nhau, hay thích làm phước, hướng thiện.</t>
+  </si>
+  <si>
+    <t>Hôn nhân hạnh phúc, vợ chồng hòa thuận và thương yêu nhau, chịu đựng được nghịch cảnh mà lòng dạ sắt son, Tình nghĩa vợ chồng bền lâu, biết nhường nhịn nhau, ít khi cãi cọ, cưới nhau về rồi sống với nhau bằng tình nghĩa.</t>
+  </si>
+  <si>
+    <t>Vợ chồng yêu nhau trong một thời gian dài mới đến hôn nhân, vợ chồng xứng nứa vừa đôi, vợ chồng có ân tình, ân nghĩa với nhau, đây cũng là bộ sao hóa giải nghiệp của Vợ Chồng vì thế cho dù có xung khắc thế nào thì cuối cùng vợ chồng cũng ở với nhau đến già.</t>
+  </si>
+  <si>
+    <t>Người hôn phối là người thiện lương, ôn hòa, hay thích làm phúc, tu tập, mặt mũi thường phúc hậu. Bạn sẵn sàng chịu đựng khổ đau vất vả để đi cùng mình tới cuối đời.</t>
+  </si>
+  <si>
+    <t>Người hôn phối là người hay làm phúc, giúp đời, được nhiều Bạn kính mến, nể trọng. Có thể làm các ngành nghề liên quan tới thầy thuốc, bác sỹ, thầy giáo</t>
   </si>
 </sst>
 </file>
@@ -14349,21 +14361,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14744,10 +14756,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:B4521"/>
+  <dimension ref="A1:F4521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4449" workbookViewId="0">
-      <selection activeCell="A4525" sqref="A4525"/>
+    <sheetView tabSelected="1" topLeftCell="A2097" workbookViewId="0">
+      <selection activeCell="D2119" sqref="D2119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14779,7 +14791,7 @@
         <v>4622</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>142</v>
       </c>
@@ -32035,7 +32047,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="2161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2161" s="1" t="s">
         <v>2158</v>
       </c>
@@ -32043,7 +32055,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="2162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2162" s="1" t="s">
         <v>2159</v>
       </c>
@@ -32051,15 +32063,27 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="2163" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="2163" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2163" s="1" t="s">
         <v>2160</v>
       </c>
       <c r="B2163" s="1" t="s">
         <v>4659</v>
       </c>
-    </row>
-    <row r="2164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C2163" s="1" t="s">
+        <v>4699</v>
+      </c>
+      <c r="D2163" s="1" t="s">
+        <v>4700</v>
+      </c>
+      <c r="E2163" s="1" t="s">
+        <v>4701</v>
+      </c>
+      <c r="F2163" s="1" t="s">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2164" s="1" t="s">
         <v>2161</v>
       </c>
@@ -32067,7 +32091,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="2165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2165" s="1" t="s">
         <v>2140</v>
       </c>
@@ -32075,7 +32099,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="2166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2166" s="1" t="s">
         <v>2141</v>
       </c>
@@ -32083,7 +32107,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="2167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2167" s="1" t="s">
         <v>2142</v>
       </c>
@@ -32091,7 +32115,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="2168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2168" s="1" t="s">
         <v>2143</v>
       </c>
@@ -32099,7 +32123,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="2169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2169" s="1" t="s">
         <v>2144</v>
       </c>
@@ -32107,7 +32131,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="2170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2170" s="1" t="s">
         <v>2145</v>
       </c>
@@ -32115,7 +32139,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="2171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2171" s="1" t="s">
         <v>2146</v>
       </c>
@@ -32123,7 +32147,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="2172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2172" s="1" t="s">
         <v>2147</v>
       </c>
@@ -32131,7 +32155,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="2173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2173" s="1" t="s">
         <v>2148</v>
       </c>
@@ -32139,7 +32163,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="2174" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="2174" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A2174" s="1" t="s">
         <v>2149</v>
       </c>
@@ -32147,7 +32171,7 @@
         <v>4659</v>
       </c>
     </row>
-    <row r="2175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2175" s="1" t="s">
         <v>2150</v>
       </c>
@@ -32155,7 +32179,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="2176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2176" s="1" t="s">
         <v>2162</v>
       </c>
@@ -48547,7 +48571,7 @@
         <v>4210</v>
       </c>
     </row>
-    <row r="4225" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4225" s="1" t="s">
         <v>4211</v>
       </c>
@@ -50947,57 +50971,57 @@
   <conditionalFormatting sqref="A145:A208">
     <cfRule type="duplicateValues" dxfId="22" priority="68"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6726:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3436:A3825 A3888:A4183">
-    <cfRule type="duplicateValues" dxfId="21" priority="108"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="110"/>
+  <conditionalFormatting sqref="A1810:A3333">
+    <cfRule type="duplicateValues" dxfId="21" priority="399"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3826:A3887">
-    <cfRule type="duplicateValues" dxfId="19" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4404 A2042 A2033:B2041 A2032 A4405:B4454 A4455:A4456 A4457:B4493 B4494:B4497 A4498:B1048576 A1:B2031 A2043:B4403">
-    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6726:A1048576 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3436:A3825 A3888:A4183">
+    <cfRule type="duplicateValues" dxfId="17" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6726:B1048576 B1:B23 B25:B84 B143 B1805:B1809 B3436:B3825 B3888:B4183 B209:B1631">
-    <cfRule type="duplicateValues" dxfId="9" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="18"/>
+  <conditionalFormatting sqref="B1556">
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3826:B3887">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="B2033:B2041 B1810:B2031 B2043:B3333">
+    <cfRule type="duplicateValues" dxfId="7" priority="395"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3200">
     <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1556">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2033:B2041 B1810:B2031 B2043:B3333">
-    <cfRule type="duplicateValues" dxfId="4" priority="395"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1810:A3333">
-    <cfRule type="duplicateValues" dxfId="3" priority="399"/>
+  <conditionalFormatting sqref="B3826:B3887">
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3836">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4204">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6726:B1048576 B1:B23 B25:B84 B143 B1805:B1809 B3436:B3825 B3888:B4183 B209:B1631">
+    <cfRule type="duplicateValues" dxfId="1" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>